<commit_message>
Added 16 tests for Tab Selects
</commit_message>
<xml_diff>
--- a/Resources/TestData/Resisdential.xlsx
+++ b/Resources/TestData/Resisdential.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Robot\Sigma\Resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Robot\DotCom\Resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6540"/>
   </bookViews>
   <sheets>
-    <sheet name="Simply" sheetId="2" r:id="rId1"/>
+    <sheet name="Headers" sheetId="2" r:id="rId1"/>
     <sheet name="Double" sheetId="1" r:id="rId2"/>
     <sheet name="Trible" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="65">
   <si>
     <t>TC_NO</t>
   </si>
@@ -220,19 +220,7 @@
     <t>22_F_Voice(DPU)_BB(50M)</t>
   </si>
   <si>
-    <t>01_F_BB(Simply50M)_FS(PMDPB)</t>
-  </si>
-  <si>
     <t>Manual_Test_Case_Folder</t>
-  </si>
-  <si>
-    <t>02_F_BB(Simply75M)_FS(50GB)</t>
-  </si>
-  <si>
-    <t>03_F_BB(Simply100M)_FS(PSU_CSID)</t>
-  </si>
-  <si>
-    <t>04_F_BB(SimplyUltra)_FS(PPB)</t>
   </si>
 </sst>
 </file>
@@ -586,7 +574,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,107 +593,59 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="4">
-        <v>46085</v>
-      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="4">
-        <v>46085</v>
-      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="4">
-        <v>46085</v>
-      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="4">
-        <v>46085</v>
-      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">

</xml_diff>

<commit_message>
Test data from excel add for Footer Test cases
</commit_message>
<xml_diff>
--- a/Resources/TestData/Resisdential.xlsx
+++ b/Resources/TestData/Resisdential.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="166">
   <si>
     <t>TC_NO</t>
   </si>
@@ -485,9 +485,6 @@
     <t>https://qat01.frontier.com/helpcenter/categories/internet/troubleshooting/speed-test</t>
   </si>
   <si>
-    <t>https://qat013.frontier.com/corporate/about-us/overview</t>
-  </si>
-  <si>
     <t>https://qat01.frontier.com/corporate/careers/overview</t>
   </si>
   <si>
@@ -515,13 +512,19 @@
     <t>Watch_TV_Url</t>
   </si>
   <si>
-    <t>qat02</t>
-  </si>
-  <si>
     <t>https://qat01.frontier.com/myfrontier-mobile-app</t>
   </si>
   <si>
     <t>http://videos.frontier.com/</t>
+  </si>
+  <si>
+    <t>qat01</t>
+  </si>
+  <si>
+    <t>https://qat01.frontier.com/corporate/about-us/overview</t>
+  </si>
+  <si>
+    <t>IE</t>
   </si>
 </sst>
 </file>
@@ -1310,10 +1313,10 @@
   <dimension ref="A1:BL17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z4" sqref="Z4"/>
+      <selection pane="bottomRight" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1321,28 +1324,29 @@
     <col min="1" max="1" width="7" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="38.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="38.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="37" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="49.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="45" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="42.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="52.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="30.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="36.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="34.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="34.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="47.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="30.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="47.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="35.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="58.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="58.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="82.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="81.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="48.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="26" style="5" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="53.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="27.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="39.140625" style="5" bestFit="1" customWidth="1"/>
@@ -1367,7 +1371,7 @@
     <col min="48" max="48" width="49.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="44.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="27.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="47.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="42.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="40.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="69.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="55.28515625" style="5" bestFit="1" customWidth="1"/>
@@ -1437,7 +1441,7 @@
         <v>47</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S1" s="12" t="s">
         <v>48</v>
@@ -1589,7 +1593,7 @@
         <v>23</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>30</v>
@@ -1672,9 +1676,11 @@
         <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="4"/>
+        <v>165</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="E3" s="6" t="s">
         <v>30</v>
       </c>
@@ -1698,7 +1704,7 @@
         <v>145</v>
       </c>
       <c r="Q3" s="22" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="R3" s="22" t="s">
         <v>49</v>
@@ -1760,9 +1766,11 @@
         <v>33</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="4"/>
+        <v>165</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="E4" s="6" t="s">
         <v>30</v>
       </c>
@@ -1801,7 +1809,7 @@
         <v>151</v>
       </c>
       <c r="Z4" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AA4" s="4"/>
       <c r="AB4" s="4"/>
@@ -1850,9 +1858,11 @@
         <v>34</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="4"/>
+        <v>165</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="E5" s="6" t="s">
         <v>30</v>
       </c>
@@ -1880,7 +1890,7 @@
       <c r="Y5" s="4"/>
       <c r="Z5" s="4"/>
       <c r="AA5" s="6" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="AB5" s="6" t="s">
         <v>57</v>
@@ -1889,16 +1899,16 @@
         <v>58</v>
       </c>
       <c r="AD5" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="AE5" s="6" t="s">
         <v>153</v>
-      </c>
-      <c r="AE5" s="6" t="s">
-        <v>154</v>
       </c>
       <c r="AF5" s="6" t="s">
         <v>59</v>
       </c>
       <c r="AG5" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AH5" s="4"/>
       <c r="AI5" s="4"/>
@@ -1940,9 +1950,11 @@
         <v>67</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="4"/>
+        <v>165</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="E6" s="6" t="s">
         <v>30</v>
       </c>
@@ -2034,9 +2046,11 @@
         <v>86</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="4"/>
+        <v>165</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="E7" s="6" t="s">
         <v>30</v>
       </c>
@@ -2126,9 +2140,11 @@
         <v>104</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="4"/>
+        <v>165</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="E8" s="6" t="s">
         <v>30</v>
       </c>
@@ -2180,7 +2196,7 @@
       <c r="AW8" s="4"/>
       <c r="AX8" s="4"/>
       <c r="AY8" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AZ8" s="4"/>
       <c r="BA8" s="4"/>
@@ -2204,9 +2220,11 @@
         <v>105</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="4"/>
+        <v>165</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="E9" s="6" t="s">
         <v>30</v>
       </c>
@@ -2259,7 +2277,7 @@
       <c r="AX9" s="4"/>
       <c r="AY9" s="4"/>
       <c r="AZ9" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BA9" s="4"/>
       <c r="BB9" s="4"/>
@@ -2282,9 +2300,11 @@
         <v>107</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="4"/>
+        <v>165</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="E10" s="6" t="s">
         <v>30</v>
       </c>
@@ -2338,7 +2358,7 @@
       <c r="AY10" s="4"/>
       <c r="AZ10" s="4"/>
       <c r="BA10" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="BB10" s="4"/>
       <c r="BC10" s="4"/>
@@ -2360,9 +2380,11 @@
         <v>108</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="4"/>
+        <v>165</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="E11" s="6" t="s">
         <v>30</v>
       </c>
@@ -2417,7 +2439,7 @@
       <c r="AZ11" s="4"/>
       <c r="BA11" s="4"/>
       <c r="BB11" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="BC11" s="4"/>
       <c r="BD11" s="4"/>
@@ -2438,9 +2460,11 @@
         <v>109</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="4"/>
+        <v>165</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="E12" s="6" t="s">
         <v>30</v>
       </c>
@@ -2496,7 +2520,7 @@
       <c r="BA12" s="4"/>
       <c r="BB12" s="4"/>
       <c r="BC12" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="BD12" s="4"/>
       <c r="BE12" s="4"/>
@@ -2516,9 +2540,11 @@
         <v>110</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="4"/>
+        <v>165</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="E13" s="6" t="s">
         <v>30</v>
       </c>
@@ -2596,9 +2622,11 @@
         <v>111</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="4"/>
+        <v>165</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="E14" s="6" t="s">
         <v>30</v>
       </c>
@@ -2674,9 +2702,11 @@
         <v>112</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="4"/>
+        <v>165</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="E15" s="6" t="s">
         <v>30</v>
       </c>
@@ -2754,9 +2784,11 @@
         <v>113</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="4"/>
+        <v>165</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="E16" s="6" t="s">
         <v>30</v>
       </c>
@@ -2834,9 +2866,11 @@
         <v>114</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="4"/>
+        <v>165</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="E17" s="6" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
modified with excel data
</commit_message>
<xml_diff>
--- a/Resources/TestData/Resisdential.xlsx
+++ b/Resources/TestData/Resisdential.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="194">
   <si>
     <t>TC_NO</t>
   </si>
@@ -507,12 +507,6 @@
   </si>
   <si>
     <t>https://qat01.frontier.com/corporate/about-us/overview</t>
-  </si>
-  <si>
-    <t>IE</t>
-  </si>
-  <si>
-    <t>Firefox</t>
   </si>
   <si>
     <t>001_CC_.COM_ENGLISH_NSS_Res_Headers_ZipCodeCheckAvailability</t>
@@ -1458,7 +1452,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P26" sqref="P26"/>
+      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,7 +1726,7 @@
         <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>161</v>
+        <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>158</v>
@@ -1818,7 +1812,7 @@
         <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>160</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>158</v>
@@ -1908,7 +1902,7 @@
         <v>28</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>160</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>158</v>
@@ -2000,7 +1994,7 @@
         <v>29</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>160</v>
+        <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>158</v>
@@ -2092,7 +2086,7 @@
         <v>62</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>160</v>
+        <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>158</v>
@@ -2188,7 +2182,7 @@
         <v>81</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>160</v>
+        <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>158</v>
@@ -2282,7 +2276,7 @@
         <v>99</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>160</v>
+        <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>158</v>
@@ -2362,7 +2356,7 @@
         <v>100</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>160</v>
+        <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>158</v>
@@ -2442,7 +2436,7 @@
         <v>102</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>160</v>
+        <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>158</v>
@@ -2522,7 +2516,7 @@
         <v>103</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>160</v>
+        <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>158</v>
@@ -2602,7 +2596,7 @@
         <v>104</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>160</v>
+        <v>18</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>158</v>
@@ -2682,7 +2676,7 @@
         <v>105</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>160</v>
+        <v>18</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>158</v>
@@ -2764,7 +2758,7 @@
         <v>106</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>160</v>
+        <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>158</v>
@@ -2844,7 +2838,7 @@
         <v>107</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>160</v>
+        <v>18</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>158</v>
@@ -2926,7 +2920,7 @@
         <v>108</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>160</v>
+        <v>18</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>158</v>
@@ -3008,7 +3002,7 @@
         <v>109</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>160</v>
+        <v>18</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>158</v>
@@ -3191,16 +3185,16 @@
         <v>138</v>
       </c>
       <c r="G1" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="J1" s="29" t="s">
         <v>177</v>
-      </c>
-      <c r="H1" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="I1" s="29" t="s">
-        <v>178</v>
-      </c>
-      <c r="J1" s="29" t="s">
-        <v>179</v>
       </c>
       <c r="K1" s="22" t="s">
         <v>22</v>
@@ -3214,7 +3208,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C2" s="24" t="s">
         <v>18</v>
@@ -3229,16 +3223,16 @@
         <v>19</v>
       </c>
       <c r="G2" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I2" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="H2" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="I2" s="26" t="s">
-        <v>173</v>
-      </c>
       <c r="J2" s="26" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K2" s="27"/>
       <c r="L2" s="25"/>
@@ -3248,7 +3242,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C3" s="24" t="s">
         <v>18</v>
@@ -3274,7 +3268,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>18</v>
@@ -3293,10 +3287,10 @@
       <c r="I4" s="24"/>
       <c r="J4" s="24"/>
       <c r="K4" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="L4" s="24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -3304,7 +3298,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>18</v>
@@ -3330,7 +3324,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>18</v>
@@ -3356,7 +3350,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C7" s="24" t="s">
         <v>18</v>
@@ -3382,7 +3376,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C8" s="24" t="s">
         <v>18</v>
@@ -3408,7 +3402,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C9" s="24" t="s">
         <v>18</v>
@@ -3434,7 +3428,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C10" s="24" t="s">
         <v>18</v>
@@ -3472,7 +3466,7 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="S1" sqref="S1"/>
@@ -3522,43 +3516,43 @@
         <v>138</v>
       </c>
       <c r="G1" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="H1" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="I1" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="J1" s="35" t="s">
         <v>183</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="K1" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="L1" s="35" t="s">
         <v>185</v>
       </c>
-      <c r="K1" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="L1" s="35" t="s">
-        <v>187</v>
-      </c>
       <c r="M1" s="35" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="N1" s="35" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="P1" s="35" t="s">
         <v>49</v>
       </c>
       <c r="Q1" s="35" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="R1" s="35" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="S1" s="35" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -3566,7 +3560,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C2" s="30" t="s">
         <v>18</v>
@@ -3872,7 +3866,7 @@
       <c r="K11" s="30"/>
       <c r="L11" s="30"/>
       <c r="M11" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="N11" s="30"/>
       <c r="O11" s="30"/>
@@ -3906,7 +3900,7 @@
       <c r="L12" s="30"/>
       <c r="M12" s="30"/>
       <c r="N12" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="O12" s="30"/>
       <c r="P12" s="30"/>

</xml_diff>

<commit_message>
Dotcom Footer section changes_5_25
</commit_message>
<xml_diff>
--- a/Resources/TestData/Resisdential.xlsx
+++ b/Resources/TestData/Resisdential.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6540" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="REG" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="228">
   <si>
     <t>TC_NO</t>
   </si>
@@ -89,9 +89,6 @@
     <t>k33p1ngITr3al</t>
   </si>
   <si>
-    <t>ftrqat03+3@gmail.com</t>
-  </si>
-  <si>
     <t>Password123</t>
   </si>
   <si>
@@ -104,9 +101,6 @@
     <t>Test_Case_Name</t>
   </si>
   <si>
-    <t>https://qat01.frontier.com/</t>
-  </si>
-  <si>
     <t>001_CC_.COM_Desktop_NSS_Res_Footers_Shop</t>
   </si>
   <si>
@@ -218,9 +212,6 @@
     <t>005_CC_.COM_Desktop_NSS_Res_Footers_FrontierSites</t>
   </si>
   <si>
-    <t>https://getvantage.com/</t>
-  </si>
-  <si>
     <t>https://ftrsecure.com/</t>
   </si>
   <si>
@@ -242,12 +233,6 @@
     <t>https://referrals.frontier.com/</t>
   </si>
   <si>
-    <t>https://business.frontier.com/become-a-partner</t>
-  </si>
-  <si>
-    <t>Business_Partner_Program_Url</t>
-  </si>
-  <si>
     <t>Referral_Program_Url</t>
   </si>
   <si>
@@ -263,9 +248,6 @@
     <t>Frontier_Games_Url</t>
   </si>
   <si>
-    <t>Frontier_BusinessEdge_Url</t>
-  </si>
-  <si>
     <t>Frontier_secure_Url</t>
   </si>
   <si>
@@ -299,30 +281,6 @@
     <t>http://west.frontier.com/</t>
   </si>
   <si>
-    <t>West_Url</t>
-  </si>
-  <si>
-    <t>SouthEast_Url</t>
-  </si>
-  <si>
-    <t>South_Url</t>
-  </si>
-  <si>
-    <t>National-ID-MT_Url</t>
-  </si>
-  <si>
-    <t>National-IL-LA-MN-NE-UT_Url</t>
-  </si>
-  <si>
-    <t>Mid_South_Url</t>
-  </si>
-  <si>
-    <t>East_Url</t>
-  </si>
-  <si>
-    <t>Central_Url</t>
-  </si>
-  <si>
     <t>Policies_Notifications</t>
   </si>
   <si>
@@ -425,90 +383,15 @@
     <t>Env</t>
   </si>
   <si>
-    <t>https://qat01.frontier.com/shop/bundles</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/shop/internet</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/shop/phone</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/shop/tv</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/shop/frontier-secure</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/corporate/movers</t>
-  </si>
-  <si>
     <t>DotCom_Url_Password</t>
   </si>
   <si>
-    <t>https://qat01.frontier.com/resources/discount-programs</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/login</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/contact-us#/residential</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/helpcenter</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/helpcenter/categories/order-status</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/helpcenter/categories/ticket-status</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/HelpCenter/SupportWizard/Troubleshoot/Sign-in/Get-Started</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/helpcenter/categories/internet/troubleshooting/speed-test</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/corporate/careers/overview</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/corporate/suppliers</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/corporate/pif/public-inspection-files</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/corporate/policies</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/corporate/terms</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/~/media/resources/policies/privacy-policy.ashx</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/corporate/retailstores/locations</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/sitemap</t>
-  </si>
-  <si>
     <t>Watch_TV_Url</t>
   </si>
   <si>
-    <t>https://qat01.frontier.com/myfrontier-mobile-app</t>
-  </si>
-  <si>
     <t>http://videos.frontier.com/</t>
   </si>
   <si>
-    <t>qat01</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/corporate/about-us/overview</t>
-  </si>
-  <si>
     <t>001_CC_.COM_ENGLISH_NSS_Res_Headers_ZipCodeCheckAvailability</t>
   </si>
   <si>
@@ -608,7 +491,226 @@
     <t>MyAccount_MyProfile_Url</t>
   </si>
   <si>
-    <t>https://qat01.frontier.com/login?target=2f6163636f756e74#/profile</t>
+    <t>ftrfrank1+automationqat02@gmail.com</t>
+  </si>
+  <si>
+    <t>Act_Num</t>
+  </si>
+  <si>
+    <t>Billing_Date</t>
+  </si>
+  <si>
+    <t>Current_Bill_Date</t>
+  </si>
+  <si>
+    <t>Total_Bill_Amount</t>
+  </si>
+  <si>
+    <t>Current_Balance</t>
+  </si>
+  <si>
+    <t>New_Charges_Due_Date</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/</t>
+  </si>
+  <si>
+    <t>425-771-3466-053185-5</t>
+  </si>
+  <si>
+    <t>Mar 19, 2017</t>
+  </si>
+  <si>
+    <t>3/19/17 - 4/18/17</t>
+  </si>
+  <si>
+    <t>$160.69</t>
+  </si>
+  <si>
+    <t>Apr 12, 2017</t>
+  </si>
+  <si>
+    <t>$140.58</t>
+  </si>
+  <si>
+    <t>Name_Button_Text</t>
+  </si>
+  <si>
+    <t>ADD PAYMENT METHOD</t>
+  </si>
+  <si>
+    <t>https://frontier.com/vantage/home</t>
+  </si>
+  <si>
+    <t>https://agents.frontier.com/</t>
+  </si>
+  <si>
+    <t>qat02</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/shop/bundles</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/shop/internet</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/shop/phone</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/shop/tv</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/shop/frontier-secure</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/corporate/movers</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/contact-us#/residential</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/helpcenter/categories/order-status</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/helpcenter/categories/ticket-status</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/HelpCenter/SupportWizard/Troubleshoot/Sign-in/Get-Started</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/login?target=2f6163636f756e74#/profile</t>
+  </si>
+  <si>
+    <t>https://frontier.com/helpcenter</t>
+  </si>
+  <si>
+    <t>Routing_Number</t>
+  </si>
+  <si>
+    <t>Bank_Accounting_Number</t>
+  </si>
+  <si>
+    <t>Re_Enter_Bank_Account_Number</t>
+  </si>
+  <si>
+    <t>021000021</t>
+  </si>
+  <si>
+    <t>9900000002</t>
+  </si>
+  <si>
+    <t>Making_A_Difference_Url</t>
+  </si>
+  <si>
+    <t>qat03</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/shop/bundles</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/shop/internet</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/shop/phone</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/shop/tv</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/shop/frontier-secure</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/corporate/movers</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/resources/discount-programs</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/login</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/myfrontier-mobile-app</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/helpcenter</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/helpcenter/SupportWizard/Troubleshoot/Sign-in/Get-Started</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/helpcenter/categories/ticket-status</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/helpcenter/categories/order-status</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/helpcenter/categories/internet/troubleshooting/speed-test</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/contact-us#/residential</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/corporate/about-us/overview</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/corporate/careers/overview</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/corporate/suppliers</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/corporate/pif/public-inspection-files</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/corporate/policies</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/corporate/terms</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/~/media/resources/policies/privacy-policy.ashx</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/corporate/retailstores/locations</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/sitemap</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/makingadifference</t>
+  </si>
+  <si>
+    <t>Frontier_Business_Url</t>
+  </si>
+  <si>
+    <t>Frontier_Business_partner_Url</t>
+  </si>
+  <si>
+    <t>Frontier_Internet_Url</t>
+  </si>
+  <si>
+    <t>Frontier_Local_Internet_Url</t>
+  </si>
+  <si>
+    <t>Frontier_Fios_Url</t>
+  </si>
+  <si>
+    <t>Frontier_Plans_Url</t>
+  </si>
+  <si>
+    <t>Frontier_Broadband_Url</t>
+  </si>
+  <si>
+    <t>Frontier_Internet_plans_Url</t>
+  </si>
+  <si>
+    <t>Frontier_Bundles_Url</t>
+  </si>
+  <si>
+    <t>Frontier_West_Url</t>
   </si>
 </sst>
 </file>
@@ -1116,10 +1218,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1128,38 +1230,78 @@
     <col min="2" max="2" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="3"/>
+    <col min="8" max="8" width="21.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="31.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1168,20 +1310,27 @@
         <v>18</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1190,16 +1339,31 @@
         <v>18</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="F3" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1208,16 +1372,43 @@
         <v>18</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F4" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1226,16 +1417,41 @@
         <v>18</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F5" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1244,16 +1460,33 @@
         <v>18</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1262,7 +1495,7 @@
         <v>18</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>19</v>
@@ -1270,8 +1503,19 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1280,7 +1524,7 @@
         <v>18</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>19</v>
@@ -1288,8 +1532,19 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1298,7 +1553,7 @@
         <v>18</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>19</v>
@@ -1306,8 +1561,19 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1316,7 +1582,7 @@
         <v>18</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>19</v>
@@ -1324,8 +1590,19 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -1334,7 +1611,7 @@
         <v>18</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>19</v>
@@ -1342,8 +1619,19 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -1352,7 +1640,7 @@
         <v>18</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>19</v>
@@ -1360,8 +1648,19 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -1370,7 +1669,7 @@
         <v>18</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>19</v>
@@ -1378,8 +1677,19 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1388,7 +1698,7 @@
         <v>18</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>19</v>
@@ -1396,8 +1706,19 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1406,7 +1727,7 @@
         <v>18</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>19</v>
@@ -1414,8 +1735,19 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -1424,7 +1756,7 @@
         <v>18</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>19</v>
@@ -1432,27 +1764,40 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3:D16" r:id="rId2" display="https://qat01.frontier.com/"/>
-    <hyperlink ref="F2" r:id="rId3"/>
+    <hyperlink ref="D2" r:id="rId1" display="https://qat01.frontier.com/"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F5" r:id="rId4"/>
+    <hyperlink ref="F6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BL17"/>
+  <dimension ref="A1:BM17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="AP2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomRight" activeCell="AR25" sqref="AR25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1476,287 +1821,291 @@
     <col min="17" max="17" width="47.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="22.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="30.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="47.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="35.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="58.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="35.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="82.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="58.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="82.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="58.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="81.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="26" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="47.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="53.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="27.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="39.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="51.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="44" style="3" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="39.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="59.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="23.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="28.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="51.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="40.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="35.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="26.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="28.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="45.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="28.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="38.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="45" style="3" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="33.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="27.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="49.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="44.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="27.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="42.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="40.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="69.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="55.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="33.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="31.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="38.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="38.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="58.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="33.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="42.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="33.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="36.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="33" style="3" bestFit="1" customWidth="1"/>
-    <col min="65" max="16384" width="6.7109375" style="3"/>
+    <col min="33" max="33" width="39.7109375" style="3" customWidth="1"/>
+    <col min="34" max="34" width="59.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="23.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="28.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="51.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="40.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="35.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="26.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="28.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="45.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="28.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="38.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="45" style="3" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="33.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="27.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="49.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="44.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="27.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="42.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="40.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="69.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="55.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="33.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="31.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="38.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="38.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="58.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="33.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="42.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="33.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="36.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="33" style="3" bestFit="1" customWidth="1"/>
+    <col min="66" max="16384" width="6.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:65" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="L1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="R1" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="S1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>43</v>
-      </c>
       <c r="T1" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="U1" s="8" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="V1" s="8" t="s">
         <v>47</v>
       </c>
       <c r="W1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="X1" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y1" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="Z1" s="8" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AA1" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AB1" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AC1" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AD1" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AE1" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AF1" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AG1" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH1" s="13" t="s">
-        <v>80</v>
+        <v>190</v>
+      </c>
+      <c r="AH1" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="AI1" s="13" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="AJ1" s="13" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="AK1" s="13" t="s">
-        <v>77</v>
+        <v>218</v>
       </c>
       <c r="AL1" s="13" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="AM1" s="13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="AN1" s="13" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="AO1" s="13" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="AP1" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="AQ1" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="AQ1" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="AR1" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="AS1" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="AT1" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="AU1" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="AV1" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AW1" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="AX1" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="AY1" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="AZ1" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="BA1" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="BB1" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="BC1" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="AR1" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="AS1" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="AT1" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AU1" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="AV1" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="AW1" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX1" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="AY1" s="6" t="s">
+      <c r="BD1" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="AZ1" s="16" t="s">
+      <c r="BE1" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="BF1" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="BA1" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="BB1" s="10" t="s">
+      <c r="BG1" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="BH1" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="BI1" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="BJ1" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="BK1" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="BC1" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="BD1" s="11" t="s">
+      <c r="BL1" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="BE1" s="11" t="s">
+      <c r="BM1" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="BF1" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="BG1" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="BH1" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="BI1" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="BJ1" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="BK1" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="BL1" s="10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>158</v>
+        <v>191</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>25</v>
+        <v>192</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>132</v>
+        <v>193</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>133</v>
+        <v>194</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>134</v>
+        <v>195</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>135</v>
+        <v>196</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>136</v>
+        <v>197</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>137</v>
+        <v>198</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>139</v>
+        <v>199</v>
       </c>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
@@ -1803,22 +2152,23 @@
       <c r="BJ2" s="2"/>
       <c r="BK2" s="2"/>
       <c r="BL2" s="2"/>
-    </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM2" s="2"/>
+    </row>
+    <row r="3" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>158</v>
+        <v>191</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>25</v>
+        <v>192</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>19</v>
@@ -1831,22 +2181,22 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="4" t="s">
-        <v>140</v>
+        <v>200</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="P3" s="20" t="s">
-        <v>140</v>
+        <v>200</v>
       </c>
       <c r="Q3" s="20" t="s">
-        <v>156</v>
+        <v>201</v>
       </c>
       <c r="R3" s="20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="S3" s="20" t="s">
-        <v>140</v>
+        <v>200</v>
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
@@ -1893,22 +2243,23 @@
       <c r="BJ3" s="2"/>
       <c r="BK3" s="2"/>
       <c r="BL3" s="2"/>
-    </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM3" s="2"/>
+    </row>
+    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>158</v>
+        <v>191</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>25</v>
+        <v>192</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>19</v>
@@ -1927,25 +2278,25 @@
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="4" t="s">
-        <v>141</v>
+        <v>202</v>
       </c>
       <c r="U4" s="4" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>143</v>
+        <v>203</v>
       </c>
       <c r="W4" s="4" t="s">
-        <v>144</v>
+        <v>204</v>
       </c>
       <c r="X4" s="4" t="s">
-        <v>145</v>
+        <v>205</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>146</v>
+        <v>206</v>
       </c>
       <c r="Z4" s="4" t="s">
-        <v>157</v>
+        <v>207</v>
       </c>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
@@ -1985,22 +2336,23 @@
       <c r="BJ4" s="2"/>
       <c r="BK4" s="2"/>
       <c r="BL4" s="2"/>
-    </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM4" s="2"/>
+    </row>
+    <row r="5" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>158</v>
+        <v>191</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>25</v>
+        <v>192</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>19</v>
@@ -2026,27 +2378,29 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
       <c r="AA5" s="4" t="s">
-        <v>159</v>
+        <v>208</v>
       </c>
       <c r="AB5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD5" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AE5" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="AF5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AC5" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AD5" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="AE5" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="AF5" s="4" t="s">
-        <v>54</v>
-      </c>
       <c r="AG5" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="AH5" s="2"/>
+        <v>217</v>
+      </c>
+      <c r="AH5" s="4" t="s">
+        <v>211</v>
+      </c>
       <c r="AI5" s="2"/>
       <c r="AJ5" s="2"/>
       <c r="AK5" s="2"/>
@@ -2077,22 +2431,23 @@
       <c r="BJ5" s="2"/>
       <c r="BK5" s="2"/>
       <c r="BL5" s="2"/>
-    </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM5" s="2"/>
+    </row>
+    <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>158</v>
+        <v>191</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>25</v>
+        <v>192</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>19</v>
@@ -2124,34 +2479,34 @@
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
       <c r="AG6" s="2"/>
-      <c r="AH6" s="4" t="s">
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="AJ6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL6" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="AI6" s="4" t="s">
+      <c r="AM6" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="AJ6" s="4" t="s">
+      <c r="AN6" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="AK6" s="4" t="s">
+      <c r="AO6" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="AL6" s="4" t="s">
+      <c r="AP6" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AM6" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN6" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AO6" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AP6" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="AQ6" s="2"/>
+      <c r="AQ6" s="4" t="s">
+        <v>171</v>
+      </c>
       <c r="AR6" s="2"/>
       <c r="AS6" s="2"/>
       <c r="AT6" s="2"/>
@@ -2173,22 +2528,23 @@
       <c r="BJ6" s="2"/>
       <c r="BK6" s="2"/>
       <c r="BL6" s="2"/>
-    </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM6" s="2"/>
+    </row>
+    <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>158</v>
+        <v>191</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>25</v>
+        <v>192</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>19</v>
@@ -2229,31 +2585,31 @@
       <c r="AN7" s="2"/>
       <c r="AO7" s="2"/>
       <c r="AP7" s="2"/>
-      <c r="AQ7" s="4" t="s">
+      <c r="AQ7" s="2"/>
+      <c r="AR7" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AS7" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT7" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="AR7" s="17" t="s">
+      <c r="AU7" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AV7" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AW7" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="AX7" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="AY7" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="AS7" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AT7" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AU7" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="AV7" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="AW7" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="AX7" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="AY7" s="2"/>
       <c r="AZ7" s="2"/>
       <c r="BA7" s="2"/>
       <c r="BB7" s="2"/>
@@ -2267,22 +2623,23 @@
       <c r="BJ7" s="2"/>
       <c r="BK7" s="2"/>
       <c r="BL7" s="2"/>
-    </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM7" s="2"/>
+    </row>
+    <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>158</v>
+        <v>191</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>25</v>
+        <v>192</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>19</v>
@@ -2331,10 +2688,10 @@
       <c r="AV8" s="2"/>
       <c r="AW8" s="2"/>
       <c r="AX8" s="2"/>
-      <c r="AY8" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="AZ8" s="2"/>
+      <c r="AY8" s="2"/>
+      <c r="AZ8" s="18" t="s">
+        <v>212</v>
+      </c>
       <c r="BA8" s="2"/>
       <c r="BB8" s="2"/>
       <c r="BC8" s="2"/>
@@ -2347,22 +2704,23 @@
       <c r="BJ8" s="2"/>
       <c r="BK8" s="2"/>
       <c r="BL8" s="2"/>
-    </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM8" s="2"/>
+    </row>
+    <row r="9" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>158</v>
+        <v>191</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>25</v>
+        <v>192</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>19</v>
@@ -2412,10 +2770,10 @@
       <c r="AW9" s="2"/>
       <c r="AX9" s="2"/>
       <c r="AY9" s="2"/>
-      <c r="AZ9" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="BA9" s="2"/>
+      <c r="AZ9" s="2"/>
+      <c r="BA9" s="4" t="s">
+        <v>213</v>
+      </c>
       <c r="BB9" s="2"/>
       <c r="BC9" s="2"/>
       <c r="BD9" s="2"/>
@@ -2427,22 +2785,23 @@
       <c r="BJ9" s="2"/>
       <c r="BK9" s="2"/>
       <c r="BL9" s="2"/>
-    </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM9" s="2"/>
+    </row>
+    <row r="10" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>158</v>
+        <v>191</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>25</v>
+        <v>192</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>19</v>
@@ -2493,10 +2852,10 @@
       <c r="AX10" s="2"/>
       <c r="AY10" s="2"/>
       <c r="AZ10" s="2"/>
-      <c r="BA10" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="BB10" s="2"/>
+      <c r="BA10" s="2"/>
+      <c r="BB10" s="4" t="s">
+        <v>214</v>
+      </c>
       <c r="BC10" s="2"/>
       <c r="BD10" s="2"/>
       <c r="BE10" s="2"/>
@@ -2507,22 +2866,23 @@
       <c r="BJ10" s="2"/>
       <c r="BK10" s="2"/>
       <c r="BL10" s="2"/>
-    </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM10" s="2"/>
+    </row>
+    <row r="11" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>158</v>
+        <v>191</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>25</v>
+        <v>192</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>19</v>
@@ -2574,10 +2934,10 @@
       <c r="AY11" s="2"/>
       <c r="AZ11" s="2"/>
       <c r="BA11" s="2"/>
-      <c r="BB11" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="BC11" s="2"/>
+      <c r="BB11" s="2"/>
+      <c r="BC11" s="4" t="s">
+        <v>215</v>
+      </c>
       <c r="BD11" s="2"/>
       <c r="BE11" s="2"/>
       <c r="BF11" s="2"/>
@@ -2587,22 +2947,23 @@
       <c r="BJ11" s="2"/>
       <c r="BK11" s="2"/>
       <c r="BL11" s="2"/>
-    </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM11" s="2"/>
+    </row>
+    <row r="12" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>158</v>
+        <v>191</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>25</v>
+        <v>192</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>19</v>
@@ -2655,10 +3016,10 @@
       <c r="AZ12" s="2"/>
       <c r="BA12" s="2"/>
       <c r="BB12" s="2"/>
-      <c r="BC12" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="BD12" s="2"/>
+      <c r="BC12" s="2"/>
+      <c r="BD12" s="4" t="s">
+        <v>216</v>
+      </c>
       <c r="BE12" s="2"/>
       <c r="BF12" s="2"/>
       <c r="BG12" s="2"/>
@@ -2667,22 +3028,23 @@
       <c r="BJ12" s="2"/>
       <c r="BK12" s="2"/>
       <c r="BL12" s="2"/>
-    </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM12" s="2"/>
+    </row>
+    <row r="13" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>158</v>
+        <v>191</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>25</v>
+        <v>192</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>19</v>
@@ -2736,35 +3098,36 @@
       <c r="BA13" s="2"/>
       <c r="BB13" s="2"/>
       <c r="BC13" s="2"/>
-      <c r="BD13" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="BE13" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="BF13" s="2"/>
+      <c r="BD13" s="2"/>
+      <c r="BE13" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="BF13" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="BG13" s="2"/>
       <c r="BH13" s="2"/>
       <c r="BI13" s="2"/>
       <c r="BJ13" s="2"/>
       <c r="BK13" s="2"/>
       <c r="BL13" s="2"/>
-    </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM13" s="2"/>
+    </row>
+    <row r="14" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>158</v>
+        <v>191</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>25</v>
+        <v>192</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>19</v>
@@ -2820,31 +3183,32 @@
       <c r="BC14" s="2"/>
       <c r="BD14" s="2"/>
       <c r="BE14" s="2"/>
-      <c r="BF14" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="BG14" s="2"/>
+      <c r="BF14" s="2"/>
+      <c r="BG14" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="BH14" s="2"/>
       <c r="BI14" s="2"/>
       <c r="BJ14" s="2"/>
       <c r="BK14" s="2"/>
       <c r="BL14" s="2"/>
-    </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM14" s="2"/>
+    </row>
+    <row r="15" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>158</v>
+        <v>191</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>25</v>
+        <v>192</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>19</v>
@@ -2901,32 +3265,33 @@
       <c r="BD15" s="2"/>
       <c r="BE15" s="2"/>
       <c r="BF15" s="2"/>
-      <c r="BG15" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="BH15" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="BI15" s="2"/>
+      <c r="BG15" s="2"/>
+      <c r="BH15" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="BI15" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="BJ15" s="2"/>
       <c r="BK15" s="2"/>
       <c r="BL15" s="2"/>
-    </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM15" s="2"/>
+    </row>
+    <row r="16" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>158</v>
+        <v>191</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>25</v>
+        <v>192</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>19</v>
@@ -2985,30 +3350,31 @@
       <c r="BF16" s="2"/>
       <c r="BG16" s="2"/>
       <c r="BH16" s="2"/>
-      <c r="BI16" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="BJ16" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="BK16" s="2"/>
+      <c r="BI16" s="2"/>
+      <c r="BJ16" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="BK16" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="BL16" s="2"/>
-    </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM16" s="2"/>
+    </row>
+    <row r="17" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>158</v>
+        <v>191</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>25</v>
+        <v>192</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>19</v>
@@ -3069,71 +3435,73 @@
       <c r="BH17" s="2"/>
       <c r="BI17" s="2"/>
       <c r="BJ17" s="2"/>
-      <c r="BK17" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="BL17" s="2" t="s">
-        <v>128</v>
+      <c r="BK17" s="2"/>
+      <c r="BL17" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="BM17" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3:E16" r:id="rId1" display="https://qat01.frontier.com/"/>
-    <hyperlink ref="E17" r:id="rId2"/>
-    <hyperlink ref="G2" r:id="rId3"/>
-    <hyperlink ref="H2" r:id="rId4"/>
-    <hyperlink ref="I2" r:id="rId5"/>
-    <hyperlink ref="J2" r:id="rId6"/>
-    <hyperlink ref="L2" r:id="rId7"/>
-    <hyperlink ref="M2" r:id="rId8"/>
-    <hyperlink ref="N3" r:id="rId9"/>
-    <hyperlink ref="T4" r:id="rId10" location="/residential"/>
-    <hyperlink ref="U4" r:id="rId11"/>
-    <hyperlink ref="V4" r:id="rId12"/>
-    <hyperlink ref="W4" r:id="rId13"/>
-    <hyperlink ref="X4" r:id="rId14"/>
-    <hyperlink ref="Y4" r:id="rId15"/>
-    <hyperlink ref="Z4" r:id="rId16"/>
-    <hyperlink ref="AA5" r:id="rId17"/>
+    <hyperlink ref="E17" r:id="rId2" display="https://qat01.frontier.com/"/>
+    <hyperlink ref="G2" r:id="rId3" display="https://qat01.frontier.com/shop/bundles"/>
+    <hyperlink ref="H2" r:id="rId4" display="https://qat01.frontier.com/shop/internet"/>
+    <hyperlink ref="I2" r:id="rId5" display="https://qat01.frontier.com/shop/phone"/>
+    <hyperlink ref="J2" r:id="rId6" display="https://qat01.frontier.com/shop/tv"/>
+    <hyperlink ref="L2" r:id="rId7" display="https://qat01.frontier.com/corporate/movers"/>
+    <hyperlink ref="M2" r:id="rId8" display="https://qat01.frontier.com/resources/discount-programs"/>
+    <hyperlink ref="N3" r:id="rId9" display="https://qat01.frontier.com/login"/>
+    <hyperlink ref="Z4" r:id="rId10" location="/residential" display="https://qat01.frontier.com/contact-us#/residential"/>
+    <hyperlink ref="T4" r:id="rId11" display="https://qat01.frontier.com/helpcenter"/>
+    <hyperlink ref="X4" r:id="rId12" display="https://qat01.frontier.com/helpcenter/categories/order-status"/>
+    <hyperlink ref="W4" r:id="rId13" display="https://qat01.frontier.com/helpcenter/categories/ticket-status"/>
+    <hyperlink ref="V4" r:id="rId14" display="https://qat02.frontier.com/helpcenter/SupportWizard/Troubleshoot/Sign-in/Get-Started"/>
+    <hyperlink ref="Y4" r:id="rId15" display="https://qat01.frontier.com/helpcenter/categories/internet/troubleshooting/speed-test"/>
+    <hyperlink ref="U4" r:id="rId16"/>
+    <hyperlink ref="AA5" r:id="rId17" display="https://qat01.frontier.com/corporate/about-us/overview"/>
     <hyperlink ref="AB5" r:id="rId18"/>
     <hyperlink ref="AC5" r:id="rId19"/>
-    <hyperlink ref="AD5" r:id="rId20"/>
-    <hyperlink ref="AE5" r:id="rId21"/>
+    <hyperlink ref="AD5" r:id="rId20" display="https://qat01.frontier.com/corporate/careers/overview"/>
+    <hyperlink ref="AE5" r:id="rId21" display="https://qat01.frontier.com/corporate/suppliers"/>
     <hyperlink ref="AF5" r:id="rId22"/>
-    <hyperlink ref="AG5" r:id="rId23"/>
-    <hyperlink ref="AH6" r:id="rId24"/>
-    <hyperlink ref="AI6" r:id="rId25"/>
-    <hyperlink ref="AJ6" r:id="rId26"/>
-    <hyperlink ref="AK6" r:id="rId27"/>
-    <hyperlink ref="AL6" r:id="rId28"/>
-    <hyperlink ref="AM6" r:id="rId29"/>
-    <hyperlink ref="AN6" r:id="rId30"/>
-    <hyperlink ref="AO6" r:id="rId31"/>
-    <hyperlink ref="AP6" r:id="rId32"/>
-    <hyperlink ref="AQ7" r:id="rId33"/>
-    <hyperlink ref="AS7" r:id="rId34"/>
-    <hyperlink ref="AT7" r:id="rId35"/>
-    <hyperlink ref="AU7" r:id="rId36"/>
-    <hyperlink ref="AV7" r:id="rId37"/>
-    <hyperlink ref="AW7" r:id="rId38"/>
-    <hyperlink ref="AZ9" r:id="rId39"/>
-    <hyperlink ref="BA10" r:id="rId40"/>
-    <hyperlink ref="BB11" r:id="rId41"/>
-    <hyperlink ref="BC12" r:id="rId42"/>
-    <hyperlink ref="BD13" r:id="rId43"/>
-    <hyperlink ref="BF14" r:id="rId44"/>
-    <hyperlink ref="BG15" r:id="rId45"/>
-    <hyperlink ref="BI16" r:id="rId46"/>
-    <hyperlink ref="BK17" r:id="rId47"/>
-    <hyperlink ref="E2" r:id="rId48"/>
-    <hyperlink ref="K2" r:id="rId49"/>
-    <hyperlink ref="P3" r:id="rId50"/>
-    <hyperlink ref="S3" r:id="rId51"/>
-    <hyperlink ref="AY8" r:id="rId52"/>
-    <hyperlink ref="R3" r:id="rId53"/>
+    <hyperlink ref="AH5" r:id="rId23" display="https://qat01.frontier.com/corporate/pif/public-inspection-files"/>
+    <hyperlink ref="AI6" r:id="rId24"/>
+    <hyperlink ref="AJ6" r:id="rId25"/>
+    <hyperlink ref="AK6" r:id="rId26"/>
+    <hyperlink ref="AL6" r:id="rId27"/>
+    <hyperlink ref="AM6" r:id="rId28"/>
+    <hyperlink ref="AN6" r:id="rId29"/>
+    <hyperlink ref="AO6" r:id="rId30"/>
+    <hyperlink ref="AP6" r:id="rId31"/>
+    <hyperlink ref="AR7" r:id="rId32"/>
+    <hyperlink ref="AT7" r:id="rId33"/>
+    <hyperlink ref="AU7" r:id="rId34"/>
+    <hyperlink ref="AV7" r:id="rId35"/>
+    <hyperlink ref="AW7" r:id="rId36"/>
+    <hyperlink ref="AX7" r:id="rId37"/>
+    <hyperlink ref="BA9" r:id="rId38" display="https://qat01.frontier.com/corporate/terms"/>
+    <hyperlink ref="BB10" r:id="rId39" display="https://qat01.frontier.com/~/media/resources/policies/privacy-policy.ashx"/>
+    <hyperlink ref="BC11" r:id="rId40" display="https://qat01.frontier.com/corporate/retailstores/locations"/>
+    <hyperlink ref="BD12" r:id="rId41" display="https://qat01.frontier.com/sitemap"/>
+    <hyperlink ref="BE13" r:id="rId42"/>
+    <hyperlink ref="BG14" r:id="rId43"/>
+    <hyperlink ref="BH15" r:id="rId44"/>
+    <hyperlink ref="BJ16" r:id="rId45"/>
+    <hyperlink ref="BL17" r:id="rId46"/>
+    <hyperlink ref="E2" r:id="rId47" display="https://qat01.frontier.com/"/>
+    <hyperlink ref="K2" r:id="rId48" display="https://qat01.frontier.com/shop/frontier-secure"/>
+    <hyperlink ref="P3" r:id="rId49" display="https://qat01.frontier.com/login"/>
+    <hyperlink ref="S3" r:id="rId50" display="https://qat01.frontier.com/login"/>
+    <hyperlink ref="AZ8" r:id="rId51" display="https://qat01.frontier.com/corporate/policies"/>
+    <hyperlink ref="R3" r:id="rId52"/>
+    <hyperlink ref="AQ6" r:id="rId53"/>
+    <hyperlink ref="AS7" r:id="rId54"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId54"/>
+  <pageSetup orientation="portrait" r:id="rId55"/>
 </worksheet>
 </file>
 
@@ -3170,37 +3538,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F1" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="J1" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="G1" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="H1" s="29" t="s">
-        <v>178</v>
-      </c>
-      <c r="I1" s="29" t="s">
-        <v>176</v>
-      </c>
-      <c r="J1" s="29" t="s">
-        <v>177</v>
-      </c>
       <c r="K1" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="22" t="s">
         <v>22</v>
-      </c>
-      <c r="L1" s="22" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -3208,31 +3576,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>160</v>
+        <v>121</v>
       </c>
       <c r="C2" s="24" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F2" s="24" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="26" t="s">
-        <v>169</v>
+        <v>130</v>
       </c>
       <c r="H2" s="26" t="s">
-        <v>172</v>
+        <v>133</v>
       </c>
       <c r="I2" s="26" t="s">
-        <v>171</v>
+        <v>132</v>
       </c>
       <c r="J2" s="26" t="s">
-        <v>170</v>
+        <v>131</v>
       </c>
       <c r="K2" s="27"/>
       <c r="L2" s="25"/>
@@ -3242,16 +3610,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="25" t="s">
         <v>161</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>25</v>
       </c>
       <c r="F3" s="24" t="s">
         <v>19</v>
@@ -3268,16 +3636,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>162</v>
+        <v>123</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>19</v>
@@ -3287,10 +3655,10 @@
       <c r="I4" s="24"/>
       <c r="J4" s="24"/>
       <c r="K4" s="4" t="s">
-        <v>173</v>
+        <v>134</v>
       </c>
       <c r="L4" s="24" t="s">
-        <v>174</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -3298,16 +3666,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>163</v>
+        <v>124</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F5" s="24" t="s">
         <v>19</v>
@@ -3324,16 +3692,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>164</v>
+        <v>125</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F6" s="24" t="s">
         <v>19</v>
@@ -3350,16 +3718,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>165</v>
+        <v>126</v>
       </c>
       <c r="C7" s="24" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F7" s="24" t="s">
         <v>19</v>
@@ -3376,16 +3744,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>166</v>
+        <v>127</v>
       </c>
       <c r="C8" s="24" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F8" s="24" t="s">
         <v>19</v>
@@ -3402,16 +3770,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>167</v>
+        <v>128</v>
       </c>
       <c r="C9" s="24" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>19</v>
@@ -3428,16 +3796,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>168</v>
+        <v>129</v>
       </c>
       <c r="C10" s="24" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F10" s="24" t="s">
         <v>19</v>
@@ -3452,8 +3820,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3:E9" r:id="rId1" display="https://qat01.frontier.com/"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="E10" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId2" display="https://qat01.frontier.com/"/>
+    <hyperlink ref="E10" r:id="rId3" display="https://qat01.frontier.com/"/>
     <hyperlink ref="K4" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3465,11 +3833,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S1" sqref="S1"/>
+      <selection pane="bottomRight" activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3501,58 +3869,58 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>180</v>
+        <v>141</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>181</v>
+        <v>142</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>182</v>
+        <v>143</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>183</v>
+        <v>144</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>184</v>
+        <v>145</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>185</v>
+        <v>146</v>
       </c>
       <c r="M1" s="35" t="s">
-        <v>192</v>
+        <v>153</v>
       </c>
       <c r="N1" s="35" t="s">
-        <v>191</v>
+        <v>152</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>190</v>
+        <v>151</v>
       </c>
       <c r="P1" s="35" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q1" s="35" t="s">
-        <v>189</v>
+        <v>150</v>
       </c>
       <c r="R1" s="35" t="s">
-        <v>188</v>
+        <v>149</v>
       </c>
       <c r="S1" s="35" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -3560,22 +3928,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>179</v>
+        <v>140</v>
       </c>
       <c r="C2" s="30" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F2" s="30" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="31" t="s">
-        <v>132</v>
+        <v>173</v>
       </c>
       <c r="H2" s="31"/>
       <c r="I2" s="31"/>
@@ -3593,17 +3961,17 @@
         <v>18</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="30"/>
       <c r="H3" s="4" t="s">
-        <v>133</v>
+        <v>174</v>
       </c>
       <c r="I3" s="30"/>
       <c r="J3" s="30"/>
@@ -3626,10 +3994,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F4" s="30" t="s">
         <v>19</v>
@@ -3637,7 +4005,7 @@
       <c r="G4" s="30"/>
       <c r="H4" s="30"/>
       <c r="I4" s="4" t="s">
-        <v>134</v>
+        <v>175</v>
       </c>
       <c r="J4" s="30"/>
       <c r="K4" s="30"/>
@@ -3659,10 +4027,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F5" s="30" t="s">
         <v>19</v>
@@ -3671,7 +4039,7 @@
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
       <c r="J5" s="5" t="s">
-        <v>135</v>
+        <v>176</v>
       </c>
       <c r="K5" s="30"/>
       <c r="L5" s="30"/>
@@ -3692,10 +4060,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F6" s="30" t="s">
         <v>19</v>
@@ -3705,7 +4073,7 @@
       <c r="I6" s="30"/>
       <c r="J6" s="30"/>
       <c r="K6" s="4" t="s">
-        <v>136</v>
+        <v>177</v>
       </c>
       <c r="L6" s="30"/>
       <c r="M6" s="30"/>
@@ -3725,10 +4093,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F7" s="30" t="s">
         <v>19</v>
@@ -3739,7 +4107,7 @@
       <c r="J7" s="30"/>
       <c r="K7" s="30"/>
       <c r="L7" s="4" t="s">
-        <v>137</v>
+        <v>178</v>
       </c>
       <c r="M7" s="30"/>
       <c r="N7" s="30"/>
@@ -3758,10 +4126,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F8" s="30" t="s">
         <v>19</v>
@@ -3789,10 +4157,10 @@
         <v>18</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F9" s="30" t="s">
         <v>19</v>
@@ -3820,10 +4188,10 @@
         <v>18</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F10" s="30" t="s">
         <v>19</v>
@@ -3851,10 +4219,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F11" s="30" t="s">
         <v>19</v>
@@ -3866,7 +4234,7 @@
       <c r="K11" s="30"/>
       <c r="L11" s="30"/>
       <c r="M11" s="4" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="N11" s="30"/>
       <c r="O11" s="30"/>
@@ -3884,10 +4252,10 @@
         <v>18</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F12" s="30" t="s">
         <v>19</v>
@@ -3900,7 +4268,7 @@
       <c r="L12" s="30"/>
       <c r="M12" s="30"/>
       <c r="N12" s="4" t="s">
-        <v>186</v>
+        <v>147</v>
       </c>
       <c r="O12" s="30"/>
       <c r="P12" s="30"/>
@@ -3917,10 +4285,10 @@
         <v>18</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F13" s="30" t="s">
         <v>19</v>
@@ -3934,7 +4302,7 @@
       <c r="M13" s="30"/>
       <c r="N13" s="30"/>
       <c r="O13" s="20" t="s">
-        <v>142</v>
+        <v>184</v>
       </c>
       <c r="P13" s="30"/>
       <c r="Q13" s="30"/>
@@ -3950,10 +4318,10 @@
         <v>18</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F14" s="30" t="s">
         <v>19</v>
@@ -3968,7 +4336,7 @@
       <c r="N14" s="30"/>
       <c r="O14" s="30"/>
       <c r="P14" s="4" t="s">
-        <v>145</v>
+        <v>182</v>
       </c>
       <c r="Q14" s="30"/>
       <c r="R14" s="30"/>
@@ -3983,10 +4351,10 @@
         <v>18</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F15" s="30" t="s">
         <v>19</v>
@@ -4002,7 +4370,7 @@
       <c r="O15" s="30"/>
       <c r="P15" s="30"/>
       <c r="Q15" s="4" t="s">
-        <v>144</v>
+        <v>181</v>
       </c>
       <c r="R15" s="30"/>
       <c r="S15" s="30"/>
@@ -4016,10 +4384,10 @@
         <v>18</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F16" s="30" t="s">
         <v>19</v>
@@ -4036,7 +4404,7 @@
       <c r="P16" s="30"/>
       <c r="Q16" s="30"/>
       <c r="R16" s="4" t="s">
-        <v>143</v>
+        <v>180</v>
       </c>
       <c r="S16" s="30"/>
     </row>
@@ -4049,10 +4417,10 @@
         <v>18</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F17" s="30" t="s">
         <v>19</v>
@@ -4070,25 +4438,25 @@
       <c r="Q17" s="30"/>
       <c r="R17" s="30"/>
       <c r="S17" s="4" t="s">
-        <v>141</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3:E16" r:id="rId1" display="https://qat01.frontier.com/"/>
-    <hyperlink ref="E17" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="G2" r:id="rId4"/>
-    <hyperlink ref="H3" r:id="rId5"/>
-    <hyperlink ref="I4" r:id="rId6"/>
-    <hyperlink ref="K6" r:id="rId7"/>
-    <hyperlink ref="L7" r:id="rId8"/>
+    <hyperlink ref="E17" r:id="rId2" display="https://qat01.frontier.com/"/>
+    <hyperlink ref="E2" r:id="rId3" display="https://qat01.frontier.com/"/>
+    <hyperlink ref="G2" r:id="rId4" display="https://qat01.frontier.com/shop/bundles"/>
+    <hyperlink ref="H3" r:id="rId5" display="https://qat01.frontier.com/shop/internet"/>
+    <hyperlink ref="I4" r:id="rId6" display="https://qat01.frontier.com/shop/phone"/>
+    <hyperlink ref="K6" r:id="rId7" display="https://qat01.frontier.com/shop/frontier-secure"/>
+    <hyperlink ref="L7" r:id="rId8" display="https://qat01.frontier.com/corporate/movers"/>
     <hyperlink ref="N12" r:id="rId9"/>
     <hyperlink ref="O13" r:id="rId10"/>
-    <hyperlink ref="P14" r:id="rId11"/>
-    <hyperlink ref="Q15" r:id="rId12"/>
-    <hyperlink ref="R16" r:id="rId13"/>
-    <hyperlink ref="S17" r:id="rId14" location="/residential"/>
+    <hyperlink ref="P14" r:id="rId11" display="https://qat01.frontier.com/HelpCenter/SupportWizard/Troubleshoot/Sign-in/Get-Started"/>
+    <hyperlink ref="Q15" r:id="rId12" display="https://qat01.frontier.com/helpcenter/categories/ticket-status"/>
+    <hyperlink ref="R16" r:id="rId13" display="https://qat01.frontier.com/helpcenter/categories/order-status"/>
+    <hyperlink ref="S17" r:id="rId14" location="/residential" display="https://qat01.frontier.com/contact-us#/residential"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId15"/>

</xml_diff>

<commit_message>
8 Reg test cases added
</commit_message>
<xml_diff>
--- a/Resources/TestData/Resisdential.xlsx
+++ b/Resources/TestData/Resisdential.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="222">
   <si>
     <t>TC_NO</t>
   </si>
@@ -491,202 +491,208 @@
     <t>MyAccount_MyProfile_Url</t>
   </si>
   <si>
+    <t>Act_Num</t>
+  </si>
+  <si>
+    <t>Billing_Date</t>
+  </si>
+  <si>
+    <t>Current_Bill_Date</t>
+  </si>
+  <si>
+    <t>Total_Bill_Amount</t>
+  </si>
+  <si>
+    <t>Current_Balance</t>
+  </si>
+  <si>
+    <t>New_Charges_Due_Date</t>
+  </si>
+  <si>
+    <t>425-771-3466-053185-5</t>
+  </si>
+  <si>
+    <t>Name_Button_Text</t>
+  </si>
+  <si>
+    <t>ADD PAYMENT METHOD</t>
+  </si>
+  <si>
+    <t>https://frontier.com/vantage/home</t>
+  </si>
+  <si>
+    <t>https://agents.frontier.com/</t>
+  </si>
+  <si>
+    <t>https://frontier.com/helpcenter</t>
+  </si>
+  <si>
+    <t>Routing_Number</t>
+  </si>
+  <si>
+    <t>Bank_Accounting_Number</t>
+  </si>
+  <si>
+    <t>Re_Enter_Bank_Account_Number</t>
+  </si>
+  <si>
+    <t>021000021</t>
+  </si>
+  <si>
+    <t>9900000002</t>
+  </si>
+  <si>
+    <t>Making_A_Difference_Url</t>
+  </si>
+  <si>
+    <t>qat03</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/shop/bundles</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/shop/internet</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/shop/phone</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/shop/tv</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/shop/frontier-secure</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/corporate/movers</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/resources/discount-programs</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/login</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/myfrontier-mobile-app</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/helpcenter</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/helpcenter/SupportWizard/Troubleshoot/Sign-in/Get-Started</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/helpcenter/categories/ticket-status</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/helpcenter/categories/order-status</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/helpcenter/categories/internet/troubleshooting/speed-test</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/contact-us#/residential</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/corporate/about-us/overview</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/corporate/careers/overview</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/corporate/suppliers</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/corporate/pif/public-inspection-files</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/corporate/policies</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/corporate/terms</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/~/media/resources/policies/privacy-policy.ashx</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/corporate/retailstores/locations</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/sitemap</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/makingadifference</t>
+  </si>
+  <si>
+    <t>Frontier_Business_Url</t>
+  </si>
+  <si>
+    <t>Frontier_Business_partner_Url</t>
+  </si>
+  <si>
+    <t>Frontier_Internet_Url</t>
+  </si>
+  <si>
+    <t>Frontier_Local_Internet_Url</t>
+  </si>
+  <si>
+    <t>Frontier_Fios_Url</t>
+  </si>
+  <si>
+    <t>Frontier_Plans_Url</t>
+  </si>
+  <si>
+    <t>Frontier_Broadband_Url</t>
+  </si>
+  <si>
+    <t>Frontier_Internet_plans_Url</t>
+  </si>
+  <si>
+    <t>Frontier_Bundles_Url</t>
+  </si>
+  <si>
+    <t>Frontier_West_Url</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/login?target=2f6163636f756e74#/profile</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/HelpCenter/SupportWizard/Troubleshoot/Sign-in/Get-Started</t>
+  </si>
+  <si>
+    <t>5039259450</t>
+  </si>
+  <si>
+    <t>3812</t>
+  </si>
+  <si>
+    <t>Billing_Act_Num</t>
+  </si>
+  <si>
+    <t>Billing_Act_Pin</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/</t>
+  </si>
+  <si>
     <t>ftrfrank1+automationqat02@gmail.com</t>
   </si>
   <si>
-    <t>Act_Num</t>
-  </si>
-  <si>
-    <t>Billing_Date</t>
-  </si>
-  <si>
-    <t>Current_Bill_Date</t>
-  </si>
-  <si>
-    <t>Total_Bill_Amount</t>
-  </si>
-  <si>
-    <t>Current_Balance</t>
-  </si>
-  <si>
-    <t>New_Charges_Due_Date</t>
-  </si>
-  <si>
-    <t>425-771-3466-053185-5</t>
-  </si>
-  <si>
-    <t>Name_Button_Text</t>
-  </si>
-  <si>
-    <t>ADD PAYMENT METHOD</t>
-  </si>
-  <si>
-    <t>https://frontier.com/vantage/home</t>
-  </si>
-  <si>
-    <t>https://agents.frontier.com/</t>
-  </si>
-  <si>
-    <t>https://frontier.com/helpcenter</t>
-  </si>
-  <si>
-    <t>Routing_Number</t>
-  </si>
-  <si>
-    <t>Bank_Accounting_Number</t>
-  </si>
-  <si>
-    <t>Re_Enter_Bank_Account_Number</t>
-  </si>
-  <si>
-    <t>021000021</t>
-  </si>
-  <si>
-    <t>9900000002</t>
-  </si>
-  <si>
-    <t>Making_A_Difference_Url</t>
-  </si>
-  <si>
-    <t>qat03</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/shop/bundles</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/shop/internet</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/shop/phone</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/shop/tv</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/shop/frontier-secure</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/corporate/movers</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/resources/discount-programs</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/login</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/myfrontier-mobile-app</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/helpcenter</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/helpcenter/SupportWizard/Troubleshoot/Sign-in/Get-Started</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/helpcenter/categories/ticket-status</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/helpcenter/categories/order-status</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/helpcenter/categories/internet/troubleshooting/speed-test</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/contact-us#/residential</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/corporate/about-us/overview</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/corporate/careers/overview</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/corporate/suppliers</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/corporate/pif/public-inspection-files</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/corporate/policies</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/corporate/terms</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/~/media/resources/policies/privacy-policy.ashx</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/corporate/retailstores/locations</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/sitemap</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/makingadifference</t>
-  </si>
-  <si>
-    <t>Frontier_Business_Url</t>
-  </si>
-  <si>
-    <t>Frontier_Business_partner_Url</t>
-  </si>
-  <si>
-    <t>Frontier_Internet_Url</t>
-  </si>
-  <si>
-    <t>Frontier_Local_Internet_Url</t>
-  </si>
-  <si>
-    <t>Frontier_Fios_Url</t>
-  </si>
-  <si>
-    <t>Frontier_Plans_Url</t>
-  </si>
-  <si>
-    <t>Frontier_Broadband_Url</t>
-  </si>
-  <si>
-    <t>Frontier_Internet_plans_Url</t>
-  </si>
-  <si>
-    <t>Frontier_Bundles_Url</t>
-  </si>
-  <si>
-    <t>Frontier_West_Url</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/login?target=2f6163636f756e74#/profile</t>
-  </si>
-  <si>
-    <t>https://qat03.frontier.com/HelpCenter/SupportWizard/Troubleshoot/Sign-in/Get-Started</t>
-  </si>
-  <si>
-    <t>5039259450</t>
-  </si>
-  <si>
-    <t>3812</t>
-  </si>
-  <si>
-    <t>Billing_Act_Num</t>
-  </si>
-  <si>
-    <t>Billing_Act_Pin</t>
-  </si>
-  <si>
-    <t>Apr 19, 2017</t>
-  </si>
-  <si>
-    <t>4/19/17 - 5/18/17</t>
-  </si>
-  <si>
-    <t>$146.71</t>
-  </si>
-  <si>
-    <t>May 15, 2017</t>
+    <t>Jun 19, 2017</t>
+  </si>
+  <si>
+    <t>6/19/17 - 7/18/17</t>
+  </si>
+  <si>
+    <t>$161.29</t>
+  </si>
+  <si>
+    <t>Jul 13, 2017</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/resources/cpni</t>
   </si>
 </sst>
 </file>
@@ -1194,13 +1200,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,7 +1214,7 @@
     <col min="1" max="1" width="7" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="3" bestFit="1" customWidth="1"/>
@@ -1222,7 +1228,7 @@
     <col min="15" max="15" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="24.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="31.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="9.140625" style="3"/>
   </cols>
@@ -1250,40 +1256,40 @@
         <v>22</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="N1" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="R1" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -1295,18 +1301,20 @@
         <v>18</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>174</v>
+        <v>215</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>154</v>
+        <v>216</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>160</v>
+      </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -1328,34 +1336,34 @@
         <v>18</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>174</v>
+        <v>215</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>154</v>
+        <v>216</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>20</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -1373,19 +1381,19 @@
         <v>18</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>174</v>
+        <v>215</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>154</v>
+        <v>216</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>20</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -1393,16 +1401,16 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O4" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="P4" s="2" t="s">
-        <v>171</v>
-      </c>
       <c r="Q4" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
@@ -1416,19 +1424,19 @@
         <v>18</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>174</v>
+        <v>215</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>154</v>
+        <v>216</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1451,19 +1459,19 @@
         <v>18</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>174</v>
+        <v>215</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>154</v>
+        <v>216</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1475,10 +1483,10 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="S6" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -1490,14 +1498,20 @@
         <v>18</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>174</v>
+        <v>215</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="F7" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>160</v>
+      </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -1519,14 +1533,20 @@
         <v>18</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>174</v>
+        <v>215</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="F8" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>160</v>
+      </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -1539,6 +1559,39 @@
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
     </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -1546,10 +1599,13 @@
     <hyperlink ref="F4" r:id="rId3"/>
     <hyperlink ref="F5" r:id="rId4"/>
     <hyperlink ref="F6" r:id="rId5"/>
-    <hyperlink ref="D8" r:id="rId6"/>
+    <hyperlink ref="F7" r:id="rId6"/>
+    <hyperlink ref="F8" r:id="rId7"/>
+    <hyperlink ref="D9" r:id="rId8"/>
+    <hyperlink ref="F9" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -1732,7 +1788,7 @@
         <v>54</v>
       </c>
       <c r="AG1" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AH1" s="12" t="s">
         <v>53</v>
@@ -1744,7 +1800,7 @@
         <v>73</v>
       </c>
       <c r="AK1" s="13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AL1" s="13" t="s">
         <v>72</v>
@@ -1762,31 +1818,31 @@
         <v>68</v>
       </c>
       <c r="AQ1" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="AR1" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="AR1" s="14" t="s">
+      <c r="AS1" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="AS1" s="14" t="s">
+      <c r="AT1" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="AT1" s="14" t="s">
+      <c r="AU1" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="AU1" s="14" t="s">
+      <c r="AV1" s="14" t="s">
         <v>205</v>
       </c>
-      <c r="AV1" s="14" t="s">
+      <c r="AW1" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="AW1" s="14" t="s">
+      <c r="AX1" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="AX1" s="14" t="s">
+      <c r="AY1" s="14" t="s">
         <v>208</v>
-      </c>
-      <c r="AY1" s="14" t="s">
-        <v>209</v>
       </c>
       <c r="AZ1" s="6" t="s">
         <v>84</v>
@@ -1842,34 +1898,34 @@
         <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="L2" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>180</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>181</v>
       </c>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
@@ -1929,10 +1985,10 @@
         <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>19</v>
@@ -1945,22 +2001,22 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>37</v>
       </c>
       <c r="P3" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q3" s="20" t="s">
         <v>182</v>
-      </c>
-      <c r="Q3" s="20" t="s">
-        <v>183</v>
       </c>
       <c r="R3" s="20" t="s">
         <v>42</v>
       </c>
       <c r="S3" s="20" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
@@ -2020,10 +2076,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>19</v>
@@ -2042,25 +2098,25 @@
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="U4" s="4" t="s">
         <v>120</v>
       </c>
       <c r="V4" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="W4" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="W4" s="4" t="s">
+      <c r="X4" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="X4" s="4" t="s">
+      <c r="Y4" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="Y4" s="4" t="s">
+      <c r="Z4" s="4" t="s">
         <v>188</v>
-      </c>
-      <c r="Z4" s="4" t="s">
-        <v>189</v>
       </c>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
@@ -2113,10 +2169,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>19</v>
@@ -2142,7 +2198,7 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
       <c r="AA5" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AB5" s="4" t="s">
         <v>50</v>
@@ -2151,19 +2207,19 @@
         <v>51</v>
       </c>
       <c r="AD5" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="AE5" s="4" t="s">
         <v>191</v>
-      </c>
-      <c r="AE5" s="4" t="s">
-        <v>192</v>
       </c>
       <c r="AF5" s="4" t="s">
         <v>52</v>
       </c>
       <c r="AG5" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AH5" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AI5" s="2"/>
       <c r="AJ5" s="2"/>
@@ -2208,10 +2264,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>19</v>
@@ -2245,7 +2301,7 @@
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
       <c r="AI6" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AJ6" s="4" t="s">
         <v>61</v>
@@ -2269,7 +2325,7 @@
         <v>67</v>
       </c>
       <c r="AQ6" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AR6" s="2"/>
       <c r="AS6" s="2"/>
@@ -2305,10 +2361,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>19</v>
@@ -2400,10 +2456,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>19</v>
@@ -2454,7 +2510,7 @@
       <c r="AX8" s="2"/>
       <c r="AY8" s="2"/>
       <c r="AZ8" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="BA8" s="2"/>
       <c r="BB8" s="2"/>
@@ -2481,10 +2537,10 @@
         <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>19</v>
@@ -2536,7 +2592,7 @@
       <c r="AY9" s="2"/>
       <c r="AZ9" s="2"/>
       <c r="BA9" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="BB9" s="2"/>
       <c r="BC9" s="2"/>
@@ -2562,10 +2618,10 @@
         <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>19</v>
@@ -2618,7 +2674,7 @@
       <c r="AZ10" s="2"/>
       <c r="BA10" s="2"/>
       <c r="BB10" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="BC10" s="2"/>
       <c r="BD10" s="2"/>
@@ -2643,10 +2699,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>19</v>
@@ -2700,7 +2756,7 @@
       <c r="BA11" s="2"/>
       <c r="BB11" s="2"/>
       <c r="BC11" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="BD11" s="2"/>
       <c r="BE11" s="2"/>
@@ -2724,10 +2780,10 @@
         <v>18</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>19</v>
@@ -2782,7 +2838,7 @@
       <c r="BB12" s="2"/>
       <c r="BC12" s="2"/>
       <c r="BD12" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="BE12" s="2"/>
       <c r="BF12" s="2"/>
@@ -2805,10 +2861,10 @@
         <v>18</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>19</v>
@@ -2888,10 +2944,10 @@
         <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>19</v>
@@ -2969,10 +3025,10 @@
         <v>18</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>19</v>
@@ -3052,10 +3108,10 @@
         <v>18</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>19</v>
@@ -3135,10 +3191,10 @@
         <v>18</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>19</v>
@@ -3346,10 +3402,10 @@
         <v>18</v>
       </c>
       <c r="D2" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" s="25" t="s">
         <v>173</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>174</v>
       </c>
       <c r="F2" s="24" t="s">
         <v>19</v>
@@ -3380,10 +3436,10 @@
         <v>18</v>
       </c>
       <c r="D3" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="25" t="s">
         <v>173</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>174</v>
       </c>
       <c r="F3" s="24" t="s">
         <v>19</v>
@@ -3406,10 +3462,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="E4" s="25" t="s">
         <v>173</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>174</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>19</v>
@@ -3436,10 +3492,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="E5" s="25" t="s">
         <v>173</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>174</v>
       </c>
       <c r="F5" s="24" t="s">
         <v>19</v>
@@ -3462,10 +3518,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="E6" s="25" t="s">
         <v>173</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>174</v>
       </c>
       <c r="F6" s="24" t="s">
         <v>19</v>
@@ -3488,10 +3544,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="E7" s="25" t="s">
         <v>173</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>174</v>
       </c>
       <c r="F7" s="24" t="s">
         <v>19</v>
@@ -3514,10 +3570,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="E8" s="25" t="s">
         <v>173</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>174</v>
       </c>
       <c r="F8" s="24" t="s">
         <v>19</v>
@@ -3540,10 +3596,10 @@
         <v>18</v>
       </c>
       <c r="D9" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="E9" s="25" t="s">
         <v>173</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>174</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>19</v>
@@ -3566,10 +3622,10 @@
         <v>18</v>
       </c>
       <c r="D10" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="E10" s="25" t="s">
         <v>173</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>174</v>
       </c>
       <c r="F10" s="24" t="s">
         <v>19</v>
@@ -3698,16 +3754,16 @@
         <v>18</v>
       </c>
       <c r="D2" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" s="31" t="s">
         <v>173</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="F2" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="31" t="s">
         <v>174</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>175</v>
       </c>
       <c r="H2" s="31"/>
       <c r="I2" s="31"/>
@@ -3725,17 +3781,17 @@
         <v>18</v>
       </c>
       <c r="D3" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="31" t="s">
         <v>173</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>174</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="30"/>
       <c r="H3" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I3" s="30"/>
       <c r="J3" s="30"/>
@@ -3758,10 +3814,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="E4" s="31" t="s">
         <v>173</v>
-      </c>
-      <c r="E4" s="31" t="s">
-        <v>174</v>
       </c>
       <c r="F4" s="30" t="s">
         <v>19</v>
@@ -3769,7 +3825,7 @@
       <c r="G4" s="30"/>
       <c r="H4" s="30"/>
       <c r="I4" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J4" s="30"/>
       <c r="K4" s="30"/>
@@ -3791,10 +3847,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="E5" s="31" t="s">
         <v>173</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>174</v>
       </c>
       <c r="F5" s="30" t="s">
         <v>19</v>
@@ -3803,7 +3859,7 @@
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
       <c r="J5" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K5" s="30"/>
       <c r="L5" s="30"/>
@@ -3824,10 +3880,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="E6" s="31" t="s">
         <v>173</v>
-      </c>
-      <c r="E6" s="31" t="s">
-        <v>174</v>
       </c>
       <c r="F6" s="30" t="s">
         <v>19</v>
@@ -3837,7 +3893,7 @@
       <c r="I6" s="30"/>
       <c r="J6" s="30"/>
       <c r="K6" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L6" s="30"/>
       <c r="M6" s="30"/>
@@ -3857,10 +3913,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="E7" s="31" t="s">
         <v>173</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>174</v>
       </c>
       <c r="F7" s="30" t="s">
         <v>19</v>
@@ -3871,7 +3927,7 @@
       <c r="J7" s="30"/>
       <c r="K7" s="30"/>
       <c r="L7" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M7" s="30"/>
       <c r="N7" s="30"/>
@@ -3890,10 +3946,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="E8" s="31" t="s">
         <v>173</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>174</v>
       </c>
       <c r="F8" s="30" t="s">
         <v>19</v>
@@ -3921,10 +3977,10 @@
         <v>18</v>
       </c>
       <c r="D9" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="E9" s="31" t="s">
         <v>173</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>174</v>
       </c>
       <c r="F9" s="30" t="s">
         <v>19</v>
@@ -3952,10 +4008,10 @@
         <v>18</v>
       </c>
       <c r="D10" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="E10" s="31" t="s">
         <v>173</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>174</v>
       </c>
       <c r="F10" s="30" t="s">
         <v>19</v>
@@ -3983,10 +4039,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="E11" s="31" t="s">
         <v>173</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>174</v>
       </c>
       <c r="F11" s="30" t="s">
         <v>19</v>
@@ -3998,7 +4054,7 @@
       <c r="K11" s="30"/>
       <c r="L11" s="30"/>
       <c r="M11" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="N11" s="30"/>
       <c r="O11" s="30"/>
@@ -4016,10 +4072,10 @@
         <v>18</v>
       </c>
       <c r="D12" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="E12" s="31" t="s">
         <v>173</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>174</v>
       </c>
       <c r="F12" s="30" t="s">
         <v>19</v>
@@ -4049,10 +4105,10 @@
         <v>18</v>
       </c>
       <c r="D13" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="E13" s="31" t="s">
         <v>173</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>174</v>
       </c>
       <c r="F13" s="30" t="s">
         <v>19</v>
@@ -4066,7 +4122,7 @@
       <c r="M13" s="30"/>
       <c r="N13" s="30"/>
       <c r="O13" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P13" s="30"/>
       <c r="Q13" s="30"/>
@@ -4082,10 +4138,10 @@
         <v>18</v>
       </c>
       <c r="D14" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="E14" s="31" t="s">
         <v>173</v>
-      </c>
-      <c r="E14" s="31" t="s">
-        <v>174</v>
       </c>
       <c r="F14" s="30" t="s">
         <v>19</v>
@@ -4100,7 +4156,7 @@
       <c r="N14" s="30"/>
       <c r="O14" s="30"/>
       <c r="P14" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Q14" s="30"/>
       <c r="R14" s="30"/>
@@ -4115,10 +4171,10 @@
         <v>18</v>
       </c>
       <c r="D15" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="E15" s="31" t="s">
         <v>173</v>
-      </c>
-      <c r="E15" s="31" t="s">
-        <v>174</v>
       </c>
       <c r="F15" s="30" t="s">
         <v>19</v>
@@ -4134,7 +4190,7 @@
       <c r="O15" s="30"/>
       <c r="P15" s="30"/>
       <c r="Q15" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="R15" s="30"/>
       <c r="S15" s="30"/>
@@ -4148,10 +4204,10 @@
         <v>18</v>
       </c>
       <c r="D16" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="E16" s="31" t="s">
         <v>173</v>
-      </c>
-      <c r="E16" s="31" t="s">
-        <v>174</v>
       </c>
       <c r="F16" s="30" t="s">
         <v>19</v>
@@ -4168,7 +4224,7 @@
       <c r="P16" s="30"/>
       <c r="Q16" s="30"/>
       <c r="R16" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="S16" s="30"/>
     </row>
@@ -4181,10 +4237,10 @@
         <v>18</v>
       </c>
       <c r="D17" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="E17" s="31" t="s">
         <v>173</v>
-      </c>
-      <c r="E17" s="31" t="s">
-        <v>174</v>
       </c>
       <c r="F17" s="30" t="s">
         <v>19</v>
@@ -4202,7 +4258,7 @@
       <c r="Q17" s="30"/>
       <c r="R17" s="30"/>
       <c r="S17" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified 8 reg test cases
</commit_message>
<xml_diff>
--- a/Resources/TestData/Resisdential.xlsx
+++ b/Resources/TestData/Resisdential.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6540" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6540"/>
   </bookViews>
   <sheets>
     <sheet name="REG" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="217">
   <si>
     <t>TC_NO</t>
   </si>
@@ -89,9 +89,6 @@
     <t>k33p1ngITr3al</t>
   </si>
   <si>
-    <t>Password123</t>
-  </si>
-  <si>
     <t>SignIn_Username</t>
   </si>
   <si>
@@ -575,108 +572,6 @@
     <t>Billing_Act_Pin</t>
   </si>
   <si>
-    <t>https://qat02.frontier.com/</t>
-  </si>
-  <si>
-    <t>ftrfrank1+automationqat02@gmail.com</t>
-  </si>
-  <si>
-    <t>Jun 19, 2017</t>
-  </si>
-  <si>
-    <t>6/19/17 - 7/18/17</t>
-  </si>
-  <si>
-    <t>$161.29</t>
-  </si>
-  <si>
-    <t>Jul 13, 2017</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/resources/cpni</t>
-  </si>
-  <si>
-    <t>qat02</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/shop/bundles</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/shop/internet</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/shop/phone</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/shop/tv</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/shop/frontier-secure</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/corporate/movers</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/login?target=2f6163636f756e74#/profile</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/helpcenter/categories/ticket-status</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/helpcenter/categories/order-status</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/contact-us#/residential</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/resources/discount-programs</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/login</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/myfrontier-mobile-app</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/helpcenter</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/helpcenter/SupportWizard/Troubleshoot/Sign-in/Get-Started</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/helpcenter/categories/internet/troubleshooting/speed-test</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/corporate/about-us/overview</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/corporate/careers/overview</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/corporate/suppliers</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/makingadifference</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/corporate/pif/public-inspection-files</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/corporate/policies</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/corporate/terms</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/~/media/resources/policies/privacy-policy.ashx</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/corporate/retailstores/locations</t>
-  </si>
-  <si>
-    <t>https://qat02.frontier.com/sitemap</t>
-  </si>
-  <si>
     <t>https://internet.frontier.com/fios.html</t>
   </si>
   <si>
@@ -684,6 +579,105 @@
   </si>
   <si>
     <t>https://go.frontier.com/</t>
+  </si>
+  <si>
+    <t>qat03</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/shop/bundles</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/shop/internet</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/shop/phone</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/shop/tv</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/shop/frontier-secure</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/corporate/movers</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/resources/discount-programs</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/login</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/myfrontier-mobile-app</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/helpcenter</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/helpcenter/SupportWizard/Troubleshoot/Sign-in/Get-Started</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/helpcenter/categories/ticket-status</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/helpcenter/categories/order-status</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/helpcenter/categories/internet/troubleshooting/speed-test</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/contact-us#/residential</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/corporate/about-us/overview</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/corporate/careers/overview</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/corporate/suppliers</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/makingadifference</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/corporate/pif/public-inspection-files</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/corporate/policies</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/corporate/terms</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/~/media/resources/policies/privacy-policy.ashx</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/corporate/retailstores/locations</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/sitemap</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/login?target=2f6163636f756e74#/profile</t>
+  </si>
+  <si>
+    <t>https://qat03.frontier.com/resources/cpni</t>
+  </si>
+  <si>
+    <t>7/19/17 - 8/18/17</t>
+  </si>
+  <si>
+    <t>$162.07</t>
+  </si>
+  <si>
+    <t>Aug 14, 2017</t>
+  </si>
+  <si>
+    <t>Jul 19, 2017</t>
   </si>
 </sst>
 </file>
@@ -1190,11 +1184,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I27" sqref="I27"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,58 +1220,58 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="N1" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>164</v>
-      </c>
       <c r="R1" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -1289,19 +1283,19 @@
         <v>18</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>183</v>
+        <v>130</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -1324,34 +1318,34 @@
         <v>18</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>183</v>
+        <v>130</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>184</v>
+        <v>216</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>185</v>
+        <v>213</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>186</v>
+        <v>214</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>186</v>
+        <v>214</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>187</v>
+        <v>215</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -1369,19 +1363,19 @@
         <v>18</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>183</v>
+        <v>130</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -1389,16 +1383,16 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="O4" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="P4" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="Q4" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
@@ -1412,19 +1406,19 @@
         <v>18</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>183</v>
+        <v>130</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1447,19 +1441,19 @@
         <v>18</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>183</v>
+        <v>130</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1471,10 +1465,10 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="S6" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -1486,19 +1480,19 @@
         <v>18</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>183</v>
+        <v>130</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1521,19 +1515,19 @@
         <v>18</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>183</v>
+        <v>130</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1556,16 +1550,16 @@
         <v>18</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>183</v>
+        <v>130</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -1582,14 +1576,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F5" r:id="rId4"/>
-    <hyperlink ref="F6" r:id="rId5"/>
-    <hyperlink ref="F7" r:id="rId6"/>
-    <hyperlink ref="F8" r:id="rId7"/>
-    <hyperlink ref="D9" r:id="rId8"/>
+    <hyperlink ref="D9" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId2"/>
+    <hyperlink ref="F3" r:id="rId3"/>
+    <hyperlink ref="F4" r:id="rId4"/>
+    <hyperlink ref="F5" r:id="rId5"/>
+    <hyperlink ref="F6" r:id="rId6"/>
+    <hyperlink ref="F7" r:id="rId7"/>
+    <hyperlink ref="F8" r:id="rId8"/>
     <hyperlink ref="F9" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1601,11 +1595,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AY2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="AU2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AY17" sqref="AY17"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1683,196 +1677,196 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="R1" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>41</v>
-      </c>
       <c r="T1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="X1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="U1" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="V1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="W1" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="X1" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y1" s="8" t="s">
-        <v>48</v>
-      </c>
       <c r="Z1" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AA1" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB1" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AC1" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AD1" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AE1" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AF1" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AG1" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="AH1" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI1" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ1" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK1" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="AH1" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI1" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="AJ1" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="AK1" s="13" t="s">
+      <c r="AL1" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM1" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN1" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="AO1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP1" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ1" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="AL1" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="AM1" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="AN1" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="AO1" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="AP1" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="AQ1" s="13" t="s">
+      <c r="AR1" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="AR1" s="14" t="s">
+      <c r="AS1" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="AS1" s="14" t="s">
+      <c r="AT1" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="AT1" s="14" t="s">
+      <c r="AU1" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="AU1" s="14" t="s">
+      <c r="AV1" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="AV1" s="14" t="s">
+      <c r="AW1" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="AW1" s="14" t="s">
+      <c r="AX1" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="AX1" s="14" t="s">
+      <c r="AY1" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="AY1" s="14" t="s">
-        <v>177</v>
-      </c>
       <c r="AZ1" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="BA1" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="BB1" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="BC1" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="BC1" s="10" t="s">
+      <c r="BD1" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="BD1" s="7" t="s">
-        <v>95</v>
-      </c>
       <c r="BE1" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="BF1" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BG1" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BH1" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="BI1" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="BJ1" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="BK1" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="BL1" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="BM1" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
@@ -1880,40 +1874,40 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="K2" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>192</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>200</v>
       </c>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
@@ -1967,16 +1961,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>19</v>
@@ -1989,22 +1983,22 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="4" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P3" s="19" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="Q3" s="19" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="R3" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S3" s="19" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
@@ -2058,16 +2052,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>19</v>
@@ -2086,13 +2080,13 @@
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="4" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="U4" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="W4" s="4" t="s">
         <v>197</v>
@@ -2101,10 +2095,10 @@
         <v>198</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="Z4" s="4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
@@ -2151,16 +2145,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>19</v>
@@ -2186,28 +2180,28 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
       <c r="AA5" s="4" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="AB5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AC5" s="4" t="s">
+      <c r="AD5" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="AE5" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="AF5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AD5" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="AE5" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="AF5" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="AG5" s="4" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="AH5" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="AI5" s="2"/>
       <c r="AJ5" s="2"/>
@@ -2246,16 +2240,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>19</v>
@@ -2289,31 +2283,31 @@
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
       <c r="AI6" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="AJ6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN6" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AO6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AP6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AQ6" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="AJ6" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="AK6" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL6" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="AM6" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="AN6" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AO6" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AP6" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="AQ6" s="4" t="s">
-        <v>161</v>
       </c>
       <c r="AR6" s="2"/>
       <c r="AS6" s="2"/>
@@ -2343,16 +2337,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>217</v>
+        <v>182</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>19</v>
@@ -2395,28 +2389,28 @@
       <c r="AP7" s="2"/>
       <c r="AQ7" s="2"/>
       <c r="AR7" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AS7" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="AS7" s="17" t="s">
+      <c r="AT7" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="AU7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AT7" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="AU7" s="4" t="s">
+      <c r="AV7" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="AV7" s="4" t="s">
+      <c r="AW7" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="AX7" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="AW7" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="AX7" s="17" t="s">
-        <v>79</v>
-      </c>
       <c r="AY7" s="17" t="s">
-        <v>218</v>
+        <v>183</v>
       </c>
       <c r="AZ7" s="2"/>
       <c r="BA7" s="2"/>
@@ -2438,16 +2432,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>19</v>
@@ -2498,7 +2492,7 @@
       <c r="AX8" s="2"/>
       <c r="AY8" s="2"/>
       <c r="AZ8" s="17" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="BA8" s="2"/>
       <c r="BB8" s="2"/>
@@ -2519,16 +2513,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>19</v>
@@ -2580,7 +2574,7 @@
       <c r="AY9" s="2"/>
       <c r="AZ9" s="2"/>
       <c r="BA9" s="4" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="BB9" s="2"/>
       <c r="BC9" s="2"/>
@@ -2600,16 +2594,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>19</v>
@@ -2662,7 +2656,7 @@
       <c r="AZ10" s="2"/>
       <c r="BA10" s="2"/>
       <c r="BB10" s="4" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="BC10" s="2"/>
       <c r="BD10" s="2"/>
@@ -2681,16 +2675,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>19</v>
@@ -2744,7 +2738,7 @@
       <c r="BA11" s="2"/>
       <c r="BB11" s="2"/>
       <c r="BC11" s="4" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="BD11" s="2"/>
       <c r="BE11" s="2"/>
@@ -2762,16 +2756,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>19</v>
@@ -2826,7 +2820,7 @@
       <c r="BB12" s="2"/>
       <c r="BC12" s="2"/>
       <c r="BD12" s="4" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="BE12" s="2"/>
       <c r="BF12" s="2"/>
@@ -2843,16 +2837,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>19</v>
@@ -2908,10 +2902,10 @@
       <c r="BC13" s="2"/>
       <c r="BD13" s="2"/>
       <c r="BE13" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="BF13" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="BF13" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="BG13" s="2"/>
       <c r="BH13" s="2"/>
@@ -2926,16 +2920,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>19</v>
@@ -2993,7 +2987,7 @@
       <c r="BE14" s="2"/>
       <c r="BF14" s="2"/>
       <c r="BG14" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BH14" s="2"/>
       <c r="BI14" s="2"/>
@@ -3007,16 +3001,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>19</v>
@@ -3075,10 +3069,10 @@
       <c r="BF15" s="2"/>
       <c r="BG15" s="2"/>
       <c r="BH15" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="BI15" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="BI15" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="BJ15" s="2"/>
       <c r="BK15" s="2"/>
@@ -3090,16 +3084,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>19</v>
@@ -3160,10 +3154,10 @@
       <c r="BH16" s="2"/>
       <c r="BI16" s="2"/>
       <c r="BJ16" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="BK16" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="BK16" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="BL16" s="2"/>
       <c r="BM16" s="2"/>
@@ -3173,16 +3167,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>19</v>
@@ -3245,10 +3239,10 @@
       <c r="BJ17" s="2"/>
       <c r="BK17" s="2"/>
       <c r="BL17" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="BM17" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="BM17" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -3266,7 +3260,7 @@
     <hyperlink ref="T4" r:id="rId11" display="https://qat01.frontier.com/helpcenter"/>
     <hyperlink ref="X4" r:id="rId12" display="https://qat01.frontier.com/helpcenter/categories/order-status"/>
     <hyperlink ref="W4" r:id="rId13" display="https://qat01.frontier.com/helpcenter/categories/ticket-status"/>
-    <hyperlink ref="V4" r:id="rId14"/>
+    <hyperlink ref="V4" r:id="rId14" display="https://qat02.frontier.com/helpcenter/SupportWizard/Troubleshoot/Sign-in/Get-Started"/>
     <hyperlink ref="Y4" r:id="rId15" display="https://qat01.frontier.com/helpcenter/categories/internet/troubleshooting/speed-test"/>
     <hyperlink ref="U4" r:id="rId16"/>
     <hyperlink ref="AA5" r:id="rId17" display="https://qat01.frontier.com/corporate/about-us/overview"/>
@@ -3347,37 +3341,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D1" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>115</v>
-      </c>
       <c r="G1" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="I1" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="I1" s="28" t="s">
+      <c r="J1" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="J1" s="28" t="s">
-        <v>135</v>
-      </c>
       <c r="K1" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="21" t="s">
         <v>21</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -3385,31 +3379,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F2" s="23" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="J2" s="25" t="s">
         <v>127</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>128</v>
       </c>
       <c r="K2" s="26"/>
       <c r="L2" s="24"/>
@@ -3419,16 +3413,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F3" s="23" t="s">
         <v>19</v>
@@ -3445,16 +3439,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C4" s="23" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F4" s="23" t="s">
         <v>19</v>
@@ -3464,10 +3458,10 @@
       <c r="I4" s="23"/>
       <c r="J4" s="23"/>
       <c r="K4" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="L4" s="23" t="s">
         <v>131</v>
-      </c>
-      <c r="L4" s="23" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -3475,16 +3469,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F5" s="23" t="s">
         <v>19</v>
@@ -3501,16 +3495,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C6" s="23" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F6" s="23" t="s">
         <v>19</v>
@@ -3527,16 +3521,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C7" s="23" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>19</v>
@@ -3553,16 +3547,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C8" s="23" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F8" s="23" t="s">
         <v>19</v>
@@ -3579,16 +3573,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C9" s="23" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>19</v>
@@ -3605,16 +3599,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C10" s="23" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F10" s="23" t="s">
         <v>19</v>
@@ -3678,58 +3672,58 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="G1" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="I1" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="J1" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="K1" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="L1" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="L1" s="34" t="s">
-        <v>143</v>
-      </c>
       <c r="M1" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N1" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O1" s="34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P1" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q1" s="34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R1" s="34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S1" s="34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -3737,22 +3731,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C2" s="29" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F2" s="29" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
@@ -3770,17 +3764,17 @@
         <v>18</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F3" s="29" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="29"/>
       <c r="H3" s="4" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="I3" s="29"/>
       <c r="J3" s="29"/>
@@ -3803,10 +3797,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F4" s="29" t="s">
         <v>19</v>
@@ -3814,7 +3808,7 @@
       <c r="G4" s="29"/>
       <c r="H4" s="29"/>
       <c r="I4" s="4" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="J4" s="29"/>
       <c r="K4" s="29"/>
@@ -3836,10 +3830,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F5" s="29" t="s">
         <v>19</v>
@@ -3848,7 +3842,7 @@
       <c r="H5" s="29"/>
       <c r="I5" s="29"/>
       <c r="J5" s="5" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="K5" s="29"/>
       <c r="L5" s="29"/>
@@ -3869,10 +3863,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F6" s="29" t="s">
         <v>19</v>
@@ -3882,7 +3876,7 @@
       <c r="I6" s="29"/>
       <c r="J6" s="29"/>
       <c r="K6" s="4" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="L6" s="29"/>
       <c r="M6" s="29"/>
@@ -3902,10 +3896,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F7" s="29" t="s">
         <v>19</v>
@@ -3916,7 +3910,7 @@
       <c r="J7" s="29"/>
       <c r="K7" s="29"/>
       <c r="L7" s="4" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="M7" s="29"/>
       <c r="N7" s="29"/>
@@ -3935,10 +3929,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F8" s="29" t="s">
         <v>19</v>
@@ -3966,10 +3960,10 @@
         <v>18</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>19</v>
@@ -3997,10 +3991,10 @@
         <v>18</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F10" s="29" t="s">
         <v>19</v>
@@ -4028,10 +4022,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F11" s="29" t="s">
         <v>19</v>
@@ -4043,7 +4037,7 @@
       <c r="K11" s="29"/>
       <c r="L11" s="29"/>
       <c r="M11" s="4" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="N11" s="29"/>
       <c r="O11" s="29"/>
@@ -4061,10 +4055,10 @@
         <v>18</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F12" s="29" t="s">
         <v>19</v>
@@ -4077,7 +4071,7 @@
       <c r="L12" s="29"/>
       <c r="M12" s="29"/>
       <c r="N12" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O12" s="29"/>
       <c r="P12" s="29"/>
@@ -4094,10 +4088,10 @@
         <v>18</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F13" s="29" t="s">
         <v>19</v>
@@ -4111,7 +4105,7 @@
       <c r="M13" s="29"/>
       <c r="N13" s="29"/>
       <c r="O13" s="19" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="P13" s="29"/>
       <c r="Q13" s="29"/>
@@ -4127,10 +4121,10 @@
         <v>18</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F14" s="29" t="s">
         <v>19</v>
@@ -4145,7 +4139,7 @@
       <c r="N14" s="29"/>
       <c r="O14" s="29"/>
       <c r="P14" s="4" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="Q14" s="29"/>
       <c r="R14" s="29"/>
@@ -4160,10 +4154,10 @@
         <v>18</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F15" s="29" t="s">
         <v>19</v>
@@ -4193,10 +4187,10 @@
         <v>18</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F16" s="29" t="s">
         <v>19</v>
@@ -4226,10 +4220,10 @@
         <v>18</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F17" s="29" t="s">
         <v>19</v>
@@ -4247,7 +4241,7 @@
       <c r="Q17" s="29"/>
       <c r="R17" s="29"/>
       <c r="S17" s="4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -4261,8 +4255,8 @@
     <hyperlink ref="K6" r:id="rId7" display="https://qat01.frontier.com/shop/frontier-secure"/>
     <hyperlink ref="L7" r:id="rId8" display="https://qat01.frontier.com/corporate/movers"/>
     <hyperlink ref="N12" r:id="rId9"/>
-    <hyperlink ref="O13" r:id="rId10"/>
-    <hyperlink ref="P14" r:id="rId11"/>
+    <hyperlink ref="O13" r:id="rId10" display="https://qat02.frontier.com/helpcenter"/>
+    <hyperlink ref="P14" r:id="rId11" display="https://qat02.frontier.com/helpcenter/SupportWizard/Troubleshoot/Sign-in/Get-Started"/>
     <hyperlink ref="Q15" r:id="rId12" display="https://qat01.frontier.com/helpcenter/categories/ticket-status"/>
     <hyperlink ref="R16" r:id="rId13" display="https://qat01.frontier.com/helpcenter/categories/order-status"/>
     <hyperlink ref="S17" r:id="rId14" location="/residential" display="https://qat01.frontier.com/contact-us#/residential"/>

</xml_diff>

<commit_message>
Fixed Failed test cases
</commit_message>
<xml_diff>
--- a/Resources/TestData/Resisdential.xlsx
+++ b/Resources/TestData/Resisdential.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Robot\DotCom\Resources\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6540" activeTab="1"/>
   </bookViews>
@@ -258,9 +263,6 @@
     <t>https://www.frontierinternet.com/</t>
   </si>
   <si>
-    <t>https://frontierbundles.com/</t>
-  </si>
-  <si>
     <t>https://www.frontierinternet.com/plans-pricing.html</t>
   </si>
   <si>
@@ -673,6 +675,9 @@
   </si>
   <si>
     <t>https://qat01.frontier.com/~/media/corporate/policies/privacy-policy.ashx</t>
+  </si>
+  <si>
+    <t>https://www.frontierbundles.com/</t>
   </si>
 </sst>
 </file>
@@ -1169,7 +1174,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1224,7 +1229,7 @@
         <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>20</v>
@@ -1233,40 +1238,40 @@
         <v>21</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="N1" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>163</v>
-      </c>
       <c r="R1" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -1278,19 +1283,19 @@
         <v>18</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -1313,34 +1318,34 @@
         <v>18</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>186</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -1358,19 +1363,19 @@
         <v>18</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="H4" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -1378,16 +1383,16 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O4" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="P4" s="2" t="s">
-        <v>165</v>
-      </c>
       <c r="Q4" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
@@ -1401,19 +1406,19 @@
         <v>18</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="H5" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1436,19 +1441,19 @@
         <v>18</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="H6" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1460,10 +1465,10 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="S6" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -1475,19 +1480,19 @@
         <v>18</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="H7" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1510,19 +1515,19 @@
         <v>18</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="H8" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1545,16 +1550,16 @@
         <v>18</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -1591,10 +1596,10 @@
   <dimension ref="A1:BM17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AY2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AT2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BB10" sqref="BB10"/>
+      <selection pane="bottomRight" activeCell="AX7" sqref="AX7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1678,13 +1683,13 @@
         <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>28</v>
@@ -1720,7 +1725,7 @@
         <v>39</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="S1" s="10" t="s">
         <v>40</v>
@@ -1765,7 +1770,7 @@
         <v>53</v>
       </c>
       <c r="AG1" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AH1" s="12" t="s">
         <v>52</v>
@@ -1777,7 +1782,7 @@
         <v>72</v>
       </c>
       <c r="AK1" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AL1" s="13" t="s">
         <v>71</v>
@@ -1795,73 +1800,73 @@
         <v>67</v>
       </c>
       <c r="AQ1" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="AR1" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="AR1" s="14" t="s">
+      <c r="AS1" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="AS1" s="14" t="s">
+      <c r="AT1" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="AT1" s="14" t="s">
+      <c r="AU1" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="AU1" s="14" t="s">
+      <c r="AV1" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="AV1" s="14" t="s">
+      <c r="AW1" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="AW1" s="14" t="s">
+      <c r="AX1" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="AX1" s="14" t="s">
+      <c r="AY1" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="AY1" s="14" t="s">
-        <v>176</v>
-      </c>
       <c r="AZ1" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BA1" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BB1" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BC1" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="BC1" s="10" t="s">
+      <c r="BD1" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="BD1" s="7" t="s">
-        <v>94</v>
-      </c>
       <c r="BE1" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BF1" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="BG1" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BH1" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="BI1" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="BJ1" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="BK1" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BL1" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="BM1" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
@@ -1875,34 +1880,34 @@
         <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="L2" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>196</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>197</v>
       </c>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
@@ -1962,10 +1967,10 @@
         <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>19</v>
@@ -1978,22 +1983,22 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>36</v>
       </c>
       <c r="P3" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q3" s="19" t="s">
         <v>198</v>
-      </c>
-      <c r="Q3" s="19" t="s">
-        <v>199</v>
       </c>
       <c r="R3" s="19" t="s">
         <v>41</v>
       </c>
       <c r="S3" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
@@ -2053,10 +2058,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>19</v>
@@ -2075,25 +2080,25 @@
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="V4" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="U4" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="V4" s="4" t="s">
+      <c r="W4" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="W4" s="4" t="s">
+      <c r="X4" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="X4" s="4" t="s">
+      <c r="Y4" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="Y4" s="4" t="s">
+      <c r="Z4" s="4" t="s">
         <v>204</v>
-      </c>
-      <c r="Z4" s="4" t="s">
-        <v>205</v>
       </c>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
@@ -2146,10 +2151,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>19</v>
@@ -2175,7 +2180,7 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
       <c r="AA5" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AB5" s="4" t="s">
         <v>49</v>
@@ -2184,19 +2189,19 @@
         <v>50</v>
       </c>
       <c r="AD5" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="AE5" s="4" t="s">
         <v>207</v>
-      </c>
-      <c r="AE5" s="4" t="s">
-        <v>208</v>
       </c>
       <c r="AF5" s="4" t="s">
         <v>51</v>
       </c>
       <c r="AG5" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="AH5" s="4" t="s">
         <v>209</v>
-      </c>
-      <c r="AH5" s="4" t="s">
-        <v>210</v>
       </c>
       <c r="AI5" s="2"/>
       <c r="AJ5" s="2"/>
@@ -2241,10 +2246,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>19</v>
@@ -2278,7 +2283,7 @@
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
       <c r="AI6" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AJ6" s="4" t="s">
         <v>60</v>
@@ -2302,7 +2307,7 @@
         <v>66</v>
       </c>
       <c r="AQ6" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AR6" s="2"/>
       <c r="AS6" s="2"/>
@@ -2332,16 +2337,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>19</v>
@@ -2390,7 +2395,7 @@
         <v>75</v>
       </c>
       <c r="AT7" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AU7" s="4" t="s">
         <v>76</v>
@@ -2399,13 +2404,13 @@
         <v>77</v>
       </c>
       <c r="AW7" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AX7" s="17" t="s">
-        <v>78</v>
+        <v>216</v>
       </c>
       <c r="AY7" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AZ7" s="2"/>
       <c r="BA7" s="2"/>
@@ -2427,16 +2432,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>19</v>
@@ -2487,7 +2492,7 @@
       <c r="AX8" s="2"/>
       <c r="AY8" s="2"/>
       <c r="AZ8" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="BA8" s="2"/>
       <c r="BB8" s="2"/>
@@ -2508,16 +2513,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>19</v>
@@ -2569,7 +2574,7 @@
       <c r="AY9" s="2"/>
       <c r="AZ9" s="2"/>
       <c r="BA9" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="BB9" s="2"/>
       <c r="BC9" s="2"/>
@@ -2589,16 +2594,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>19</v>
@@ -2651,7 +2656,7 @@
       <c r="AZ10" s="2"/>
       <c r="BA10" s="2"/>
       <c r="BB10" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="BC10" s="2"/>
       <c r="BD10" s="2"/>
@@ -2670,16 +2675,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>19</v>
@@ -2733,7 +2738,7 @@
       <c r="BA11" s="2"/>
       <c r="BB11" s="2"/>
       <c r="BC11" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="BD11" s="2"/>
       <c r="BE11" s="2"/>
@@ -2751,16 +2756,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>19</v>
@@ -2815,7 +2820,7 @@
       <c r="BB12" s="2"/>
       <c r="BC12" s="2"/>
       <c r="BD12" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="BE12" s="2"/>
       <c r="BF12" s="2"/>
@@ -2832,16 +2837,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>19</v>
@@ -2897,10 +2902,10 @@
       <c r="BC13" s="2"/>
       <c r="BD13" s="2"/>
       <c r="BE13" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="BF13" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="BF13" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="BG13" s="2"/>
       <c r="BH13" s="2"/>
@@ -2915,16 +2920,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>19</v>
@@ -2982,7 +2987,7 @@
       <c r="BE14" s="2"/>
       <c r="BF14" s="2"/>
       <c r="BG14" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="BH14" s="2"/>
       <c r="BI14" s="2"/>
@@ -2996,16 +3001,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>19</v>
@@ -3064,10 +3069,10 @@
       <c r="BF15" s="2"/>
       <c r="BG15" s="2"/>
       <c r="BH15" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="BI15" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="BI15" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="BJ15" s="2"/>
       <c r="BK15" s="2"/>
@@ -3079,16 +3084,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>19</v>
@@ -3149,10 +3154,10 @@
       <c r="BH16" s="2"/>
       <c r="BI16" s="2"/>
       <c r="BJ16" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="BK16" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="BK16" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="BL16" s="2"/>
       <c r="BM16" s="2"/>
@@ -3162,16 +3167,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>19</v>
@@ -3234,10 +3239,10 @@
       <c r="BJ17" s="2"/>
       <c r="BK17" s="2"/>
       <c r="BL17" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="BM17" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="BM17" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -3342,25 +3347,25 @@
         <v>17</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E1" s="20" t="s">
         <v>27</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G1" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="H1" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="I1" s="28" t="s">
+      <c r="J1" s="28" t="s">
         <v>133</v>
-      </c>
-      <c r="J1" s="28" t="s">
-        <v>134</v>
       </c>
       <c r="K1" s="21" t="s">
         <v>20</v>
@@ -3374,31 +3379,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F2" s="23" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="J2" s="25" t="s">
         <v>126</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>127</v>
       </c>
       <c r="K2" s="26"/>
       <c r="L2" s="24"/>
@@ -3408,16 +3413,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F3" s="23" t="s">
         <v>19</v>
@@ -3434,16 +3439,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4" s="23" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F4" s="23" t="s">
         <v>19</v>
@@ -3453,10 +3458,10 @@
       <c r="I4" s="23"/>
       <c r="J4" s="23"/>
       <c r="K4" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="L4" s="23" t="s">
         <v>130</v>
-      </c>
-      <c r="L4" s="23" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -3464,16 +3469,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F5" s="23" t="s">
         <v>19</v>
@@ -3490,16 +3495,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C6" s="23" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F6" s="23" t="s">
         <v>19</v>
@@ -3516,16 +3521,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C7" s="23" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>19</v>
@@ -3542,16 +3547,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C8" s="23" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F8" s="23" t="s">
         <v>19</v>
@@ -3568,16 +3573,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" s="23" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>19</v>
@@ -3594,16 +3599,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C10" s="23" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F10" s="23" t="s">
         <v>19</v>
@@ -3673,52 +3678,52 @@
         <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G1" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="I1" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="J1" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="K1" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="L1" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="L1" s="34" t="s">
-        <v>142</v>
-      </c>
       <c r="M1" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N1" s="34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O1" s="34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P1" s="34" t="s">
         <v>46</v>
       </c>
       <c r="Q1" s="34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R1" s="34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="S1" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -3726,22 +3731,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C2" s="29" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="30" t="s">
         <v>190</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>188</v>
-      </c>
-      <c r="F2" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>191</v>
       </c>
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
@@ -3759,17 +3764,17 @@
         <v>18</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F3" s="29" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="29"/>
       <c r="H3" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I3" s="29"/>
       <c r="J3" s="29"/>
@@ -3792,10 +3797,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F4" s="29" t="s">
         <v>19</v>
@@ -3803,7 +3808,7 @@
       <c r="G4" s="29"/>
       <c r="H4" s="29"/>
       <c r="I4" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J4" s="29"/>
       <c r="K4" s="29"/>
@@ -3825,10 +3830,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F5" s="29" t="s">
         <v>19</v>
@@ -3837,7 +3842,7 @@
       <c r="H5" s="29"/>
       <c r="I5" s="29"/>
       <c r="J5" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K5" s="29"/>
       <c r="L5" s="29"/>
@@ -3858,10 +3863,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F6" s="29" t="s">
         <v>19</v>
@@ -3871,7 +3876,7 @@
       <c r="I6" s="29"/>
       <c r="J6" s="29"/>
       <c r="K6" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L6" s="29"/>
       <c r="M6" s="29"/>
@@ -3891,10 +3896,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F7" s="29" t="s">
         <v>19</v>
@@ -3905,7 +3910,7 @@
       <c r="J7" s="29"/>
       <c r="K7" s="29"/>
       <c r="L7" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M7" s="29"/>
       <c r="N7" s="29"/>
@@ -3924,10 +3929,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F8" s="29" t="s">
         <v>19</v>
@@ -3955,10 +3960,10 @@
         <v>18</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>19</v>
@@ -3986,10 +3991,10 @@
         <v>18</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F10" s="29" t="s">
         <v>19</v>
@@ -4017,10 +4022,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F11" s="29" t="s">
         <v>19</v>
@@ -4032,7 +4037,7 @@
       <c r="K11" s="29"/>
       <c r="L11" s="29"/>
       <c r="M11" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N11" s="29"/>
       <c r="O11" s="29"/>
@@ -4050,10 +4055,10 @@
         <v>18</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F12" s="29" t="s">
         <v>19</v>
@@ -4066,7 +4071,7 @@
       <c r="L12" s="29"/>
       <c r="M12" s="29"/>
       <c r="N12" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O12" s="29"/>
       <c r="P12" s="29"/>
@@ -4083,10 +4088,10 @@
         <v>18</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F13" s="29" t="s">
         <v>19</v>
@@ -4100,7 +4105,7 @@
       <c r="M13" s="29"/>
       <c r="N13" s="29"/>
       <c r="O13" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="P13" s="29"/>
       <c r="Q13" s="29"/>
@@ -4116,10 +4121,10 @@
         <v>18</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F14" s="29" t="s">
         <v>19</v>
@@ -4134,7 +4139,7 @@
       <c r="N14" s="29"/>
       <c r="O14" s="29"/>
       <c r="P14" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Q14" s="29"/>
       <c r="R14" s="29"/>
@@ -4149,10 +4154,10 @@
         <v>18</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F15" s="29" t="s">
         <v>19</v>
@@ -4168,7 +4173,7 @@
       <c r="O15" s="29"/>
       <c r="P15" s="29"/>
       <c r="Q15" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="R15" s="29"/>
       <c r="S15" s="29"/>
@@ -4182,10 +4187,10 @@
         <v>18</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F16" s="29" t="s">
         <v>19</v>
@@ -4202,7 +4207,7 @@
       <c r="P16" s="29"/>
       <c r="Q16" s="29"/>
       <c r="R16" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="S16" s="29"/>
     </row>
@@ -4215,10 +4220,10 @@
         <v>18</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F17" s="29" t="s">
         <v>19</v>
@@ -4236,7 +4241,7 @@
       <c r="Q17" s="29"/>
       <c r="R17" s="29"/>
       <c r="S17" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Headers logout issue
</commit_message>
<xml_diff>
--- a/Resources/TestData/Resisdential.xlsx
+++ b/Resources/TestData/Resisdential.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6540" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6540"/>
   </bookViews>
   <sheets>
     <sheet name="REG" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="219">
   <si>
     <t>TC_NO</t>
   </si>
@@ -578,18 +578,6 @@
     <t>https://go.frontier.com/</t>
   </si>
   <si>
-    <t>7/19/17 - 8/18/17</t>
-  </si>
-  <si>
-    <t>$162.07</t>
-  </si>
-  <si>
-    <t>Aug 14, 2017</t>
-  </si>
-  <si>
-    <t>Jul 19, 2017</t>
-  </si>
-  <si>
     <t>https://qat01.frontier.com/</t>
   </si>
   <si>
@@ -678,6 +666,24 @@
   </si>
   <si>
     <t>https://www.frontierbundles.com/</t>
+  </si>
+  <si>
+    <t>Ftrfrank1+automationtest01@gmail.com</t>
+  </si>
+  <si>
+    <t>813-986-4707-110714-5</t>
+  </si>
+  <si>
+    <t>Oct 17, 2017</t>
+  </si>
+  <si>
+    <t>$719.95</t>
+  </si>
+  <si>
+    <t>Oct 11, 2017</t>
+  </si>
+  <si>
+    <t>10/17/17 - 11/16/17</t>
   </si>
 </sst>
 </file>
@@ -1184,11 +1190,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,7 +1289,7 @@
         <v>18</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>19</v>
@@ -1318,34 +1324,34 @@
         <v>18</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>129</v>
+        <v>213</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>130</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>155</v>
+        <v>214</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>186</v>
+        <v>215</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>183</v>
+        <v>218</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>184</v>
+        <v>216</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>184</v>
+        <v>216</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>185</v>
+        <v>217</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -1363,7 +1369,7 @@
         <v>18</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>19</v>
@@ -1406,7 +1412,7 @@
         <v>18</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>19</v>
@@ -1441,7 +1447,7 @@
         <v>18</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>19</v>
@@ -1480,7 +1486,7 @@
         <v>18</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>19</v>
@@ -1515,7 +1521,7 @@
         <v>18</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>19</v>
@@ -1550,7 +1556,7 @@
         <v>18</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>19</v>
@@ -1595,8 +1601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AT2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="AX7" sqref="AX7"/>
@@ -1880,34 +1886,34 @@
         <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="K2" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>192</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>196</v>
       </c>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
@@ -1967,10 +1973,10 @@
         <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>19</v>
@@ -1983,22 +1989,22 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="4" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>36</v>
       </c>
       <c r="P3" s="19" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="Q3" s="19" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="R3" s="19" t="s">
         <v>41</v>
       </c>
       <c r="S3" s="19" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
@@ -2058,10 +2064,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>19</v>
@@ -2080,25 +2086,25 @@
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="4" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="U4" s="4" t="s">
         <v>115</v>
       </c>
       <c r="V4" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="Z4" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="X4" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="Y4" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="Z4" s="4" t="s">
-        <v>204</v>
       </c>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
@@ -2151,10 +2157,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>19</v>
@@ -2180,7 +2186,7 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
       <c r="AA5" s="4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="AB5" s="4" t="s">
         <v>49</v>
@@ -2189,19 +2195,19 @@
         <v>50</v>
       </c>
       <c r="AD5" s="4" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="AE5" s="4" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="AF5" s="4" t="s">
         <v>51</v>
       </c>
       <c r="AG5" s="4" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="AH5" s="4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="AI5" s="2"/>
       <c r="AJ5" s="2"/>
@@ -2246,10 +2252,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>19</v>
@@ -2343,10 +2349,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>19</v>
@@ -2407,7 +2413,7 @@
         <v>78</v>
       </c>
       <c r="AX7" s="17" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="AY7" s="17" t="s">
         <v>182</v>
@@ -2438,10 +2444,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>19</v>
@@ -2492,7 +2498,7 @@
       <c r="AX8" s="2"/>
       <c r="AY8" s="2"/>
       <c r="AZ8" s="17" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="BA8" s="2"/>
       <c r="BB8" s="2"/>
@@ -2519,10 +2525,10 @@
         <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>19</v>
@@ -2574,7 +2580,7 @@
       <c r="AY9" s="2"/>
       <c r="AZ9" s="2"/>
       <c r="BA9" s="4" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="BB9" s="2"/>
       <c r="BC9" s="2"/>
@@ -2600,10 +2606,10 @@
         <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>19</v>
@@ -2656,7 +2662,7 @@
       <c r="AZ10" s="2"/>
       <c r="BA10" s="2"/>
       <c r="BB10" s="4" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="BC10" s="2"/>
       <c r="BD10" s="2"/>
@@ -2681,10 +2687,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>19</v>
@@ -2738,7 +2744,7 @@
       <c r="BA11" s="2"/>
       <c r="BB11" s="2"/>
       <c r="BC11" s="4" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="BD11" s="2"/>
       <c r="BE11" s="2"/>
@@ -2762,10 +2768,10 @@
         <v>18</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>19</v>
@@ -2820,7 +2826,7 @@
       <c r="BB12" s="2"/>
       <c r="BC12" s="2"/>
       <c r="BD12" s="4" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="BE12" s="2"/>
       <c r="BF12" s="2"/>
@@ -2843,10 +2849,10 @@
         <v>18</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>19</v>
@@ -2926,10 +2932,10 @@
         <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>19</v>
@@ -3007,10 +3013,10 @@
         <v>18</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>19</v>
@@ -3090,10 +3096,10 @@
         <v>18</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>19</v>
@@ -3173,10 +3179,10 @@
         <v>18</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>19</v>
@@ -3385,10 +3391,10 @@
         <v>18</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F2" s="23" t="s">
         <v>19</v>
@@ -3419,10 +3425,10 @@
         <v>18</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F3" s="23" t="s">
         <v>19</v>
@@ -3445,10 +3451,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F4" s="23" t="s">
         <v>19</v>
@@ -3475,10 +3481,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F5" s="23" t="s">
         <v>19</v>
@@ -3501,10 +3507,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F6" s="23" t="s">
         <v>19</v>
@@ -3527,10 +3533,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>19</v>
@@ -3553,10 +3559,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F8" s="23" t="s">
         <v>19</v>
@@ -3579,10 +3585,10 @@
         <v>18</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>19</v>
@@ -3605,10 +3611,10 @@
         <v>18</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F10" s="23" t="s">
         <v>19</v>
@@ -3637,7 +3643,7 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="P14" sqref="P14"/>
@@ -3737,16 +3743,16 @@
         <v>18</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F2" s="29" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
@@ -3764,17 +3770,17 @@
         <v>18</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F3" s="29" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="29"/>
       <c r="H3" s="4" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="I3" s="29"/>
       <c r="J3" s="29"/>
@@ -3797,10 +3803,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F4" s="29" t="s">
         <v>19</v>
@@ -3808,7 +3814,7 @@
       <c r="G4" s="29"/>
       <c r="H4" s="29"/>
       <c r="I4" s="4" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="J4" s="29"/>
       <c r="K4" s="29"/>
@@ -3830,10 +3836,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F5" s="29" t="s">
         <v>19</v>
@@ -3842,7 +3848,7 @@
       <c r="H5" s="29"/>
       <c r="I5" s="29"/>
       <c r="J5" s="5" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="K5" s="29"/>
       <c r="L5" s="29"/>
@@ -3863,10 +3869,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F6" s="29" t="s">
         <v>19</v>
@@ -3876,7 +3882,7 @@
       <c r="I6" s="29"/>
       <c r="J6" s="29"/>
       <c r="K6" s="4" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="L6" s="29"/>
       <c r="M6" s="29"/>
@@ -3896,10 +3902,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F7" s="29" t="s">
         <v>19</v>
@@ -3910,7 +3916,7 @@
       <c r="J7" s="29"/>
       <c r="K7" s="29"/>
       <c r="L7" s="4" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="M7" s="29"/>
       <c r="N7" s="29"/>
@@ -3929,10 +3935,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F8" s="29" t="s">
         <v>19</v>
@@ -3960,10 +3966,10 @@
         <v>18</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>19</v>
@@ -3991,10 +3997,10 @@
         <v>18</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F10" s="29" t="s">
         <v>19</v>
@@ -4022,10 +4028,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F11" s="29" t="s">
         <v>19</v>
@@ -4037,7 +4043,7 @@
       <c r="K11" s="29"/>
       <c r="L11" s="29"/>
       <c r="M11" s="4" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="N11" s="29"/>
       <c r="O11" s="29"/>
@@ -4055,10 +4061,10 @@
         <v>18</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F12" s="29" t="s">
         <v>19</v>
@@ -4088,10 +4094,10 @@
         <v>18</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F13" s="29" t="s">
         <v>19</v>
@@ -4105,7 +4111,7 @@
       <c r="M13" s="29"/>
       <c r="N13" s="29"/>
       <c r="O13" s="19" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="P13" s="29"/>
       <c r="Q13" s="29"/>
@@ -4121,10 +4127,10 @@
         <v>18</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F14" s="29" t="s">
         <v>19</v>
@@ -4139,7 +4145,7 @@
       <c r="N14" s="29"/>
       <c r="O14" s="29"/>
       <c r="P14" s="4" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="Q14" s="29"/>
       <c r="R14" s="29"/>
@@ -4154,10 +4160,10 @@
         <v>18</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F15" s="29" t="s">
         <v>19</v>
@@ -4173,7 +4179,7 @@
       <c r="O15" s="29"/>
       <c r="P15" s="29"/>
       <c r="Q15" s="4" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="R15" s="29"/>
       <c r="S15" s="29"/>
@@ -4187,10 +4193,10 @@
         <v>18</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F16" s="29" t="s">
         <v>19</v>
@@ -4207,7 +4213,7 @@
       <c r="P16" s="29"/>
       <c r="Q16" s="29"/>
       <c r="R16" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="S16" s="29"/>
     </row>
@@ -4220,10 +4226,10 @@
         <v>18</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F17" s="29" t="s">
         <v>19</v>
@@ -4241,7 +4247,7 @@
       <c r="Q17" s="29"/>
       <c r="R17" s="29"/>
       <c r="S17" s="4" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified sheet for qat02
</commit_message>
<xml_diff>
--- a/Resources/TestData/Resisdential.xlsx
+++ b/Resources/TestData/Resisdential.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="217">
   <si>
     <t>TC_NO</t>
   </si>
@@ -416,9 +416,6 @@
     <t>Plano TX (change)</t>
   </si>
   <si>
-    <t>ftrfrank1+automation@gmail.com</t>
-  </si>
-  <si>
     <t>Frontier999</t>
   </si>
   <si>
@@ -494,9 +491,6 @@
     <t>New_Charges_Due_Date</t>
   </si>
   <si>
-    <t>425-771-3466-053185-5</t>
-  </si>
-  <si>
     <t>Name_Button_Text</t>
   </si>
   <si>
@@ -572,99 +566,9 @@
     <t>https://go.frontier.com/</t>
   </si>
   <si>
-    <t>https://qat01.frontier.com/</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/resources/cpni</t>
-  </si>
-  <si>
-    <t>qat01</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/shop/bundles</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/shop/internet</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/shop/phone</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/shop/tv</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/shop/frontier-secure</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/corporate/movers</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/resources/discount-programs</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/login</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/myfrontier-mobile-app</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/helpcenter</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/helpcenter/SupportWizard/Troubleshoot/Sign-in/Get-Started</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/helpcenter/categories/ticket-status</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/helpcenter/categories/order-status</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/helpcenter/categories/internet/troubleshooting/speed-test</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/contact-us#/residential</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/corporate/about-us/overview</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/corporate/careers/overview</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/corporate/suppliers</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/makingadifference</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/corporate/pif/public-inspection-files</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/corporate/policies</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/corporate/terms</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/corporate/retailstores/locations</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/sitemap</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/login?target=2f6163636f756e74#/profile</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/~/media/corporate/policies/privacy-policy.ashx</t>
-  </si>
-  <si>
     <t>https://www.frontierbundles.com/</t>
   </si>
   <si>
-    <t>Ftrfrank1+automationtest01@gmail.com</t>
-  </si>
-  <si>
     <t>Oct 17, 2017</t>
   </si>
   <si>
@@ -677,13 +581,103 @@
     <t>10/17/17 - 11/16/17</t>
   </si>
   <si>
-    <t xml:space="preserve">7278494301 </t>
-  </si>
-  <si>
-    <t>7557</t>
-  </si>
-  <si>
-    <t>813-986-4707-110714-5</t>
+    <t>https://qat02.frontier.com/</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/resources/cpni</t>
+  </si>
+  <si>
+    <t>qat02</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/shop/bundles</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/shop/internet</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/shop/phone</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/shop/tv</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/shop/frontier-secure</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/corporate/movers</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/resources/discount-programs</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/login</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/myfrontier-mobile-app</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/helpcenter</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/helpcenter/SupportWizard/Troubleshoot/Sign-in/Get-Started</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/helpcenter/categories/ticket-status</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/helpcenter/categories/order-status</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/helpcenter/categories/internet/troubleshooting/speed-test</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/contact-us#/residential</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/corporate/about-us/overview</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/corporate/careers/overview</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/corporate/suppliers</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/makingadifference</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/corporate/pif/public-inspection-files</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/corporate/policies</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/corporate/terms</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/~/media/corporate/policies/privacy-policy.ashx</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/corporate/retailstores/locations</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/sitemap</t>
+  </si>
+  <si>
+    <t>https://qat02.frontier.com/login?target=2f6163636f756e74#/profile</t>
+  </si>
+  <si>
+    <t>321-165-9438-031215-5</t>
+  </si>
+  <si>
+    <t>81398647071107145</t>
+  </si>
+  <si>
+    <t>9191</t>
+  </si>
+  <si>
+    <t>ftrfrank1+automation2@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1194,7 +1188,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,40 +1238,40 @@
         <v>21</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>156</v>
-      </c>
       <c r="O1" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>162</v>
-      </c>
       <c r="R1" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -1289,19 +1283,19 @@
         <v>18</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>155</v>
+        <v>213</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -1324,34 +1318,34 @@
         <v>18</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>213</v>
-      </c>
       <c r="L3" s="2" t="s">
-        <v>213</v>
+        <v>181</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>214</v>
+        <v>182</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -1369,19 +1363,19 @@
         <v>18</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="H4" s="2" t="s">
-        <v>155</v>
+        <v>213</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -1389,16 +1383,16 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
@@ -1412,19 +1406,19 @@
         <v>18</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="H5" s="2" t="s">
-        <v>155</v>
+        <v>213</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1447,19 +1441,19 @@
         <v>18</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1471,10 +1465,10 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -1486,19 +1480,19 @@
         <v>18</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1521,19 +1515,19 @@
         <v>18</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="H8" s="2" t="s">
-        <v>155</v>
+        <v>213</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1556,16 +1550,16 @@
         <v>18</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -1584,17 +1578,10 @@
   <hyperlinks>
     <hyperlink ref="D9" r:id="rId1" display="https://qat03.frontier.com/resources/cpni"/>
     <hyperlink ref="F2" r:id="rId2"/>
-    <hyperlink ref="F3" r:id="rId3"/>
-    <hyperlink ref="F4" r:id="rId4"/>
-    <hyperlink ref="F8" r:id="rId5"/>
-    <hyperlink ref="F9" r:id="rId6"/>
-    <hyperlink ref="F6" r:id="rId7"/>
-    <hyperlink ref="F7" r:id="rId8"/>
-    <hyperlink ref="F5" r:id="rId9"/>
-    <hyperlink ref="D2" r:id="rId10"/>
+    <hyperlink ref="D2" r:id="rId3" display="https://qat01.frontier.com/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1603,10 +1590,10 @@
   <dimension ref="A1:BM17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="BJ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AX7" sqref="AX7"/>
+      <selection pane="bottomRight" activeCell="BQ17" sqref="BQ17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1777,7 +1764,7 @@
         <v>53</v>
       </c>
       <c r="AG1" s="12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AH1" s="12" t="s">
         <v>52</v>
@@ -1789,7 +1776,7 @@
         <v>72</v>
       </c>
       <c r="AK1" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AL1" s="13" t="s">
         <v>71</v>
@@ -1807,31 +1794,31 @@
         <v>67</v>
       </c>
       <c r="AQ1" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="AR1" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="AS1" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="AR1" s="14" t="s">
+      <c r="AT1" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="AS1" s="14" t="s">
+      <c r="AU1" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="AT1" s="14" t="s">
+      <c r="AV1" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="AU1" s="14" t="s">
+      <c r="AW1" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="AV1" s="14" t="s">
+      <c r="AX1" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="AW1" s="14" t="s">
+      <c r="AY1" s="14" t="s">
         <v>173</v>
-      </c>
-      <c r="AX1" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="AY1" s="14" t="s">
-        <v>175</v>
       </c>
       <c r="AZ1" s="6" t="s">
         <v>79</v>
@@ -1887,34 +1874,34 @@
         <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
@@ -1974,10 +1961,10 @@
         <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>19</v>
@@ -1990,22 +1977,22 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="4" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>36</v>
       </c>
       <c r="P3" s="19" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="Q3" s="19" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="R3" s="19" t="s">
         <v>41</v>
       </c>
       <c r="S3" s="19" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
@@ -2065,10 +2052,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>19</v>
@@ -2087,25 +2074,25 @@
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="4" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="U4" s="4" t="s">
         <v>115</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="W4" s="4" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="X4" s="4" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="Z4" s="4" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
@@ -2158,10 +2145,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>19</v>
@@ -2187,7 +2174,7 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
       <c r="AA5" s="4" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AB5" s="4" t="s">
         <v>49</v>
@@ -2196,19 +2183,19 @@
         <v>50</v>
       </c>
       <c r="AD5" s="4" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="AE5" s="4" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="AF5" s="4" t="s">
         <v>51</v>
       </c>
       <c r="AG5" s="4" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AH5" s="4" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="AI5" s="2"/>
       <c r="AJ5" s="2"/>
@@ -2253,10 +2240,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>19</v>
@@ -2290,7 +2277,7 @@
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
       <c r="AI6" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AJ6" s="4" t="s">
         <v>60</v>
@@ -2314,7 +2301,7 @@
         <v>66</v>
       </c>
       <c r="AQ6" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AR6" s="2"/>
       <c r="AS6" s="2"/>
@@ -2344,16 +2331,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>19</v>
@@ -2402,7 +2389,7 @@
         <v>75</v>
       </c>
       <c r="AT7" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AU7" s="4" t="s">
         <v>76</v>
@@ -2414,10 +2401,10 @@
         <v>78</v>
       </c>
       <c r="AX7" s="17" t="s">
-        <v>210</v>
+        <v>179</v>
       </c>
       <c r="AY7" s="17" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="AZ7" s="2"/>
       <c r="BA7" s="2"/>
@@ -2445,10 +2432,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>19</v>
@@ -2499,7 +2486,7 @@
       <c r="AX8" s="2"/>
       <c r="AY8" s="2"/>
       <c r="AZ8" s="17" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="BA8" s="2"/>
       <c r="BB8" s="2"/>
@@ -2526,10 +2513,10 @@
         <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>19</v>
@@ -2581,7 +2568,7 @@
       <c r="AY9" s="2"/>
       <c r="AZ9" s="2"/>
       <c r="BA9" s="4" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="BB9" s="2"/>
       <c r="BC9" s="2"/>
@@ -2607,10 +2594,10 @@
         <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>19</v>
@@ -2688,10 +2675,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>19</v>
@@ -2745,7 +2732,7 @@
       <c r="BA11" s="2"/>
       <c r="BB11" s="2"/>
       <c r="BC11" s="4" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="BD11" s="2"/>
       <c r="BE11" s="2"/>
@@ -2769,10 +2756,10 @@
         <v>18</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>19</v>
@@ -2827,7 +2814,7 @@
       <c r="BB12" s="2"/>
       <c r="BC12" s="2"/>
       <c r="BD12" s="4" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="BE12" s="2"/>
       <c r="BF12" s="2"/>
@@ -2850,10 +2837,10 @@
         <v>18</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>19</v>
@@ -2933,10 +2920,10 @@
         <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>19</v>
@@ -3014,10 +3001,10 @@
         <v>18</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>19</v>
@@ -3097,10 +3084,10 @@
         <v>18</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>19</v>
@@ -3180,10 +3167,10 @@
         <v>18</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>19</v>
@@ -3255,28 +3242,28 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3:E16" r:id="rId1" display="https://qat01.frontier.com/"/>
-    <hyperlink ref="E17" r:id="rId2"/>
-    <hyperlink ref="G2" r:id="rId3"/>
-    <hyperlink ref="H2" r:id="rId4"/>
-    <hyperlink ref="I2" r:id="rId5"/>
-    <hyperlink ref="J2" r:id="rId6"/>
-    <hyperlink ref="L2" r:id="rId7"/>
-    <hyperlink ref="M2" r:id="rId8"/>
-    <hyperlink ref="N3" r:id="rId9"/>
-    <hyperlink ref="Z4" r:id="rId10" location="/residential"/>
-    <hyperlink ref="T4" r:id="rId11"/>
-    <hyperlink ref="X4" r:id="rId12"/>
-    <hyperlink ref="W4" r:id="rId13"/>
-    <hyperlink ref="V4" r:id="rId14" display="https://qat02.frontier.com/helpcenter/SupportWizard/Troubleshoot/Sign-in/Get-Started"/>
-    <hyperlink ref="Y4" r:id="rId15"/>
+    <hyperlink ref="E17" r:id="rId2" display="https://qat01.frontier.com/"/>
+    <hyperlink ref="G2" r:id="rId3" display="https://qat01.frontier.com/shop/bundles"/>
+    <hyperlink ref="H2" r:id="rId4" display="https://qat01.frontier.com/shop/internet"/>
+    <hyperlink ref="I2" r:id="rId5" display="https://qat01.frontier.com/shop/phone"/>
+    <hyperlink ref="J2" r:id="rId6" display="https://qat01.frontier.com/shop/tv"/>
+    <hyperlink ref="L2" r:id="rId7" display="https://qat01.frontier.com/corporate/movers"/>
+    <hyperlink ref="M2" r:id="rId8" display="https://qat01.frontier.com/resources/discount-programs"/>
+    <hyperlink ref="N3" r:id="rId9" display="https://qat01.frontier.com/login"/>
+    <hyperlink ref="Z4" r:id="rId10" location="/residential" display="https://qat01.frontier.com/contact-us#/residential"/>
+    <hyperlink ref="T4" r:id="rId11" display="https://qat01.frontier.com/helpcenter"/>
+    <hyperlink ref="X4" r:id="rId12" display="https://qat01.frontier.com/helpcenter/categories/order-status"/>
+    <hyperlink ref="W4" r:id="rId13" display="https://qat01.frontier.com/helpcenter/categories/ticket-status"/>
+    <hyperlink ref="V4" r:id="rId14"/>
+    <hyperlink ref="Y4" r:id="rId15" display="https://qat01.frontier.com/helpcenter/categories/internet/troubleshooting/speed-test"/>
     <hyperlink ref="U4" r:id="rId16"/>
-    <hyperlink ref="AA5" r:id="rId17"/>
+    <hyperlink ref="AA5" r:id="rId17" display="https://qat01.frontier.com/corporate/about-us/overview"/>
     <hyperlink ref="AB5" r:id="rId18"/>
     <hyperlink ref="AC5" r:id="rId19"/>
-    <hyperlink ref="AD5" r:id="rId20"/>
-    <hyperlink ref="AE5" r:id="rId21"/>
+    <hyperlink ref="AD5" r:id="rId20" display="https://qat01.frontier.com/corporate/careers/overview"/>
+    <hyperlink ref="AE5" r:id="rId21" display="https://qat01.frontier.com/corporate/suppliers"/>
     <hyperlink ref="AF5" r:id="rId22"/>
-    <hyperlink ref="AH5" r:id="rId23"/>
+    <hyperlink ref="AH5" r:id="rId23" display="https://qat01.frontier.com/corporate/pif/public-inspection-files"/>
     <hyperlink ref="AI6" r:id="rId24"/>
     <hyperlink ref="AJ6" r:id="rId25"/>
     <hyperlink ref="AK6" r:id="rId26"/>
@@ -3291,20 +3278,20 @@
     <hyperlink ref="AV7" r:id="rId35"/>
     <hyperlink ref="AW7" r:id="rId36"/>
     <hyperlink ref="AX7" r:id="rId37"/>
-    <hyperlink ref="BA9" r:id="rId38"/>
-    <hyperlink ref="BB10" r:id="rId39"/>
-    <hyperlink ref="BC11" r:id="rId40"/>
-    <hyperlink ref="BD12" r:id="rId41"/>
+    <hyperlink ref="BA9" r:id="rId38" display="https://qat01.frontier.com/corporate/terms"/>
+    <hyperlink ref="BB10" r:id="rId39" display="https://qat01.frontier.com/~/media/corporate/policies/privacy-policy.ashx"/>
+    <hyperlink ref="BC11" r:id="rId40" display="https://qat01.frontier.com/corporate/retailstores/locations"/>
+    <hyperlink ref="BD12" r:id="rId41" display="https://qat01.frontier.com/sitemap"/>
     <hyperlink ref="BE13" r:id="rId42"/>
     <hyperlink ref="BG14" r:id="rId43"/>
     <hyperlink ref="BH15" r:id="rId44"/>
     <hyperlink ref="BJ16" r:id="rId45"/>
     <hyperlink ref="BL17" r:id="rId46"/>
-    <hyperlink ref="E2" r:id="rId47"/>
-    <hyperlink ref="K2" r:id="rId48"/>
-    <hyperlink ref="P3" r:id="rId49"/>
-    <hyperlink ref="S3" r:id="rId50"/>
-    <hyperlink ref="AZ8" r:id="rId51"/>
+    <hyperlink ref="E2" r:id="rId47" display="https://qat01.frontier.com/"/>
+    <hyperlink ref="K2" r:id="rId48" display="https://qat01.frontier.com/shop/frontier-secure"/>
+    <hyperlink ref="P3" r:id="rId49" display="https://qat01.frontier.com/login"/>
+    <hyperlink ref="S3" r:id="rId50" display="https://qat01.frontier.com/login"/>
+    <hyperlink ref="AZ8" r:id="rId51" display="https://qat01.frontier.com/corporate/policies"/>
     <hyperlink ref="R3" r:id="rId52"/>
     <hyperlink ref="AQ6" r:id="rId53"/>
     <hyperlink ref="AS7" r:id="rId54"/>
@@ -3323,7 +3310,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3363,16 +3350,16 @@
         <v>113</v>
       </c>
       <c r="G1" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="I1" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="H1" s="28" t="s">
-        <v>134</v>
-      </c>
-      <c r="I1" s="28" t="s">
+      <c r="J1" s="28" t="s">
         <v>132</v>
-      </c>
-      <c r="J1" s="28" t="s">
-        <v>133</v>
       </c>
       <c r="K1" s="21" t="s">
         <v>20</v>
@@ -3392,10 +3379,10 @@
         <v>18</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F2" s="23" t="s">
         <v>19</v>
@@ -3426,10 +3413,10 @@
         <v>18</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F3" s="23" t="s">
         <v>19</v>
@@ -3452,10 +3439,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F4" s="23" t="s">
         <v>19</v>
@@ -3465,10 +3452,10 @@
       <c r="I4" s="23"/>
       <c r="J4" s="23"/>
       <c r="K4" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="L4" s="23" t="s">
         <v>129</v>
-      </c>
-      <c r="L4" s="23" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -3482,10 +3469,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F5" s="23" t="s">
         <v>19</v>
@@ -3508,10 +3495,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F6" s="23" t="s">
         <v>19</v>
@@ -3534,10 +3521,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>19</v>
@@ -3560,10 +3547,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F8" s="23" t="s">
         <v>19</v>
@@ -3586,10 +3573,10 @@
         <v>18</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>19</v>
@@ -3612,10 +3599,10 @@
         <v>18</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F10" s="23" t="s">
         <v>19</v>
@@ -3630,8 +3617,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3:E9" r:id="rId1" display="https://qat01.frontier.com/"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="E10" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId2" display="https://qat01.frontier.com/"/>
+    <hyperlink ref="E10" r:id="rId3" display="https://qat01.frontier.com/"/>
     <hyperlink ref="K4" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3644,10 +3631,10 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P14" sqref="P14"/>
+      <selection pane="bottomRight" activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3694,43 +3681,43 @@
         <v>113</v>
       </c>
       <c r="G1" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="I1" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="J1" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="K1" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="L1" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="L1" s="34" t="s">
-        <v>141</v>
-      </c>
       <c r="M1" s="34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N1" s="34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O1" s="34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="P1" s="34" t="s">
         <v>46</v>
       </c>
       <c r="Q1" s="34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="R1" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="S1" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -3738,22 +3725,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2" s="29" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F2" s="29" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
@@ -3771,17 +3758,17 @@
         <v>18</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F3" s="29" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="29"/>
       <c r="H3" s="4" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="I3" s="29"/>
       <c r="J3" s="29"/>
@@ -3804,10 +3791,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F4" s="29" t="s">
         <v>19</v>
@@ -3815,7 +3802,7 @@
       <c r="G4" s="29"/>
       <c r="H4" s="29"/>
       <c r="I4" s="4" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="J4" s="29"/>
       <c r="K4" s="29"/>
@@ -3837,10 +3824,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F5" s="29" t="s">
         <v>19</v>
@@ -3849,7 +3836,7 @@
       <c r="H5" s="29"/>
       <c r="I5" s="29"/>
       <c r="J5" s="5" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="K5" s="29"/>
       <c r="L5" s="29"/>
@@ -3870,10 +3857,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F6" s="29" t="s">
         <v>19</v>
@@ -3883,7 +3870,7 @@
       <c r="I6" s="29"/>
       <c r="J6" s="29"/>
       <c r="K6" s="4" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="L6" s="29"/>
       <c r="M6" s="29"/>
@@ -3903,10 +3890,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F7" s="29" t="s">
         <v>19</v>
@@ -3917,7 +3904,7 @@
       <c r="J7" s="29"/>
       <c r="K7" s="29"/>
       <c r="L7" s="4" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="M7" s="29"/>
       <c r="N7" s="29"/>
@@ -3936,10 +3923,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F8" s="29" t="s">
         <v>19</v>
@@ -3967,10 +3954,10 @@
         <v>18</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>19</v>
@@ -3998,10 +3985,10 @@
         <v>18</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F10" s="29" t="s">
         <v>19</v>
@@ -4029,10 +4016,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F11" s="29" t="s">
         <v>19</v>
@@ -4044,7 +4031,7 @@
       <c r="K11" s="29"/>
       <c r="L11" s="29"/>
       <c r="M11" s="4" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="N11" s="29"/>
       <c r="O11" s="29"/>
@@ -4062,10 +4049,10 @@
         <v>18</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F12" s="29" t="s">
         <v>19</v>
@@ -4078,7 +4065,7 @@
       <c r="L12" s="29"/>
       <c r="M12" s="29"/>
       <c r="N12" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O12" s="29"/>
       <c r="P12" s="29"/>
@@ -4095,10 +4082,10 @@
         <v>18</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F13" s="29" t="s">
         <v>19</v>
@@ -4112,7 +4099,7 @@
       <c r="M13" s="29"/>
       <c r="N13" s="29"/>
       <c r="O13" s="19" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="P13" s="29"/>
       <c r="Q13" s="29"/>
@@ -4128,10 +4115,10 @@
         <v>18</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F14" s="29" t="s">
         <v>19</v>
@@ -4146,7 +4133,7 @@
       <c r="N14" s="29"/>
       <c r="O14" s="29"/>
       <c r="P14" s="4" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="Q14" s="29"/>
       <c r="R14" s="29"/>
@@ -4161,10 +4148,10 @@
         <v>18</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F15" s="29" t="s">
         <v>19</v>
@@ -4180,7 +4167,7 @@
       <c r="O15" s="29"/>
       <c r="P15" s="29"/>
       <c r="Q15" s="4" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="R15" s="29"/>
       <c r="S15" s="29"/>
@@ -4194,10 +4181,10 @@
         <v>18</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F16" s="29" t="s">
         <v>19</v>
@@ -4214,7 +4201,7 @@
       <c r="P16" s="29"/>
       <c r="Q16" s="29"/>
       <c r="R16" s="4" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="S16" s="29"/>
     </row>
@@ -4227,10 +4214,10 @@
         <v>18</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F17" s="29" t="s">
         <v>19</v>
@@ -4248,25 +4235,25 @@
       <c r="Q17" s="29"/>
       <c r="R17" s="29"/>
       <c r="S17" s="4" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3:E16" r:id="rId1" display="https://qat01.frontier.com/"/>
-    <hyperlink ref="E17" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="G2" r:id="rId4"/>
-    <hyperlink ref="H3" r:id="rId5"/>
-    <hyperlink ref="I4" r:id="rId6"/>
-    <hyperlink ref="K6" r:id="rId7"/>
-    <hyperlink ref="L7" r:id="rId8"/>
+    <hyperlink ref="E17" r:id="rId2" display="https://qat01.frontier.com/"/>
+    <hyperlink ref="E2" r:id="rId3" display="https://qat01.frontier.com/"/>
+    <hyperlink ref="G2" r:id="rId4" display="https://qat01.frontier.com/shop/bundles"/>
+    <hyperlink ref="H3" r:id="rId5" display="https://qat01.frontier.com/shop/internet"/>
+    <hyperlink ref="I4" r:id="rId6" display="https://qat01.frontier.com/shop/phone"/>
+    <hyperlink ref="K6" r:id="rId7" display="https://qat01.frontier.com/shop/frontier-secure"/>
+    <hyperlink ref="L7" r:id="rId8" display="https://qat01.frontier.com/corporate/movers"/>
     <hyperlink ref="N12" r:id="rId9"/>
-    <hyperlink ref="O13" r:id="rId10" display="https://qat02.frontier.com/helpcenter"/>
-    <hyperlink ref="P14" r:id="rId11" display="https://qat02.frontier.com/helpcenter/SupportWizard/Troubleshoot/Sign-in/Get-Started"/>
-    <hyperlink ref="Q15" r:id="rId12"/>
-    <hyperlink ref="R16" r:id="rId13"/>
-    <hyperlink ref="S17" r:id="rId14" location="/residential"/>
+    <hyperlink ref="O13" r:id="rId10"/>
+    <hyperlink ref="P14" r:id="rId11"/>
+    <hyperlink ref="Q15" r:id="rId12" display="https://qat01.frontier.com/helpcenter/categories/ticket-status"/>
+    <hyperlink ref="R16" r:id="rId13" display="https://qat01.frontier.com/helpcenter/categories/order-status"/>
+    <hyperlink ref="S17" r:id="rId14" location="/residential" display="https://qat01.frontier.com/contact-us#/residential"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId15"/>

</xml_diff>

<commit_message>
Fixed all Frontier Secure issues
</commit_message>
<xml_diff>
--- a/Resources/TestData/Resisdential.xlsx
+++ b/Resources/TestData/Resisdential.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6540" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="REG" sheetId="4" r:id="rId1"/>
@@ -1187,11 +1187,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3633,11 +3633,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U2" sqref="U2"/>
+      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3872,7 +3872,7 @@
       <c r="H6" s="29"/>
       <c r="I6" s="29"/>
       <c r="J6" s="29"/>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="37" t="s">
         <v>187</v>
       </c>
       <c r="L6" s="29"/>
@@ -4249,7 +4249,7 @@
     <hyperlink ref="G2" r:id="rId4" display="https://qat01.frontier.com/shop/bundles"/>
     <hyperlink ref="H3" r:id="rId5" display="https://qat01.frontier.com/shop/internet"/>
     <hyperlink ref="I4" r:id="rId6" display="https://qat01.frontier.com/shop/phone"/>
-    <hyperlink ref="K6" r:id="rId7" display="https://qat01.frontier.com/shop/frontier-secure"/>
+    <hyperlink ref="K6" r:id="rId7"/>
     <hyperlink ref="L7" r:id="rId8" display="https://qat01.frontier.com/corporate/movers"/>
     <hyperlink ref="N12" r:id="rId9"/>
     <hyperlink ref="O13" r:id="rId10"/>

</xml_diff>